<commit_message>
Small changes to detection input constants; plus a few more tests run
</commit_message>
<xml_diff>
--- a/detection-test-log.xlsx
+++ b/detection-test-log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a00ae3f07a1e700d/Documents/01_Repo/Tennis-Court-Detection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="650" documentId="8_{2D7FC5CA-3D0C-4B5A-B7FB-375324B2700F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2BA7730A-4C14-4474-8571-737B6D4744F6}"/>
+  <xr:revisionPtr revIDLastSave="110" documentId="14_{49F20441-C236-4DE0-9B16-124974D818CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2BD59B5C-CBDB-4676-BE08-4942F2D4DF80}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model_Comparison" sheetId="8" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="69">
   <si>
     <t>Comments</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Model accuracy</t>
   </si>
   <si>
-    <t>Model Comparison: Parameters and Accuracy</t>
-  </si>
-  <si>
     <t>(# of images in training data)</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
     <t>Set2b</t>
   </si>
   <si>
-    <t>Set2b: manually added more pos and negs. Also processed images to duplicate each multiple times with small rotations. Positive image usage % set to 90% due to BadArgumentError (?). Image dimensions 60 x 114</t>
-  </si>
-  <si>
     <t>MinNeighbors</t>
   </si>
   <si>
@@ -200,12 +194,60 @@
   <si>
     <t>False positives were very close to the tennis court (one was in between two)</t>
   </si>
+  <si>
+    <t>Set2b: manually added more pos and negs. Also processed images to duplicate each multiple times with small rotations. Positive image usage % set to 90% due to BadArgumentError (?). Image dimensions 60 x 114. Required leaf false alarm rate achieved after 6 stages (auto-stop)</t>
+  </si>
+  <si>
+    <t>Set3</t>
+  </si>
+  <si>
+    <t>Negatives rotated at 0, 45, 90, 180, etc. (pos -2, 0, 2, 178, 180, 182). Pos img 90%. Image dimensions 60 x 114. Required leaf false alarm rate achieved after 8 stages (auto-stop)</t>
+  </si>
+  <si>
+    <t>cascade5.xml</t>
+  </si>
+  <si>
+    <t>Extra notes</t>
+  </si>
+  <si>
+    <t>Too many false positives!</t>
+  </si>
+  <si>
+    <t>Model Comparison: Parameters and Effect</t>
+  </si>
+  <si>
+    <t>Effectiveness of Each Model Iteration</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>HAAR</t>
+  </si>
+  <si>
+    <t>LBP</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>ScaleFactor</t>
+  </si>
+  <si>
+    <t>Ned to ensure min size &gt; 100 else detects a lot of FP</t>
+  </si>
+  <si>
+    <t>Both FPs can be negated with a scaleFactor of 1.5</t>
+  </si>
+  <si>
+    <t>cascade6.xml</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,8 +323,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,6 +384,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF1E8F8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -468,7 +524,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -590,6 +646,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -622,17 +680,1012 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Model_Comparison!$Q$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Precision</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Model_Comparison!$B$8:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Model_Comparison!$Q$8:$Q$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8.3333333333333329E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17647058823529413</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.20833333333333334</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.28125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A83D-4867-9DAA-1491D15BE15E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Model_Comparison!$R$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Recall</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Model_Comparison!$B$8:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Model_Comparison!$R$8:$R$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>9.0909090909090912E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.27272727272727271</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.45454545454545453</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.81818181818181823</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.72727272727272729</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A83D-4867-9DAA-1491D15BE15E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="688870096"/>
+        <c:axId val="688872336"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="688870096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="688872336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="688872336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="688870096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>1702858</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>10695</xdr:rowOff>
@@ -666,6 +1719,42 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>34926</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>41273</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{826D0F32-17B8-45D2-B336-B43277F1EC38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1017,9 +2106,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B95065D9-21E2-4631-8E00-95D37F7A67C6}">
-  <dimension ref="B1:U19"/>
+  <dimension ref="B1:X26"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1027,28 +2116,31 @@
     <col min="2" max="2" width="3.6328125" customWidth="1"/>
     <col min="3" max="3" width="12.6328125" customWidth="1"/>
     <col min="4" max="4" width="8.6328125" customWidth="1"/>
-    <col min="5" max="9" width="10.6328125" customWidth="1"/>
-    <col min="10" max="11" width="15.6328125" customWidth="1"/>
-    <col min="12" max="14" width="14.6328125" customWidth="1"/>
-    <col min="15" max="16" width="15.6328125" customWidth="1"/>
-    <col min="17" max="20" width="12.6328125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="40.6328125" customWidth="1" collapsed="1"/>
-    <col min="22" max="24" width="12.6328125" customWidth="1"/>
+    <col min="5" max="8" width="9.6328125" customWidth="1"/>
+    <col min="9" max="10" width="8.6328125" customWidth="1"/>
+    <col min="11" max="11" width="13.6328125" customWidth="1"/>
+    <col min="12" max="12" width="14.6328125" customWidth="1"/>
+    <col min="13" max="14" width="13.6328125" customWidth="1"/>
+    <col min="15" max="16" width="14.6328125" customWidth="1"/>
+    <col min="17" max="18" width="12.6328125" customWidth="1"/>
+    <col min="19" max="22" width="12.6328125" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="40.6328125" customWidth="1"/>
+    <col min="24" max="26" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:24" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="B1" s="11" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
     </row>
-    <row r="2" spans="2:21" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:24" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:24" x14ac:dyDescent="0.35">
       <c r="E4" s="20" t="s">
         <v>18</v>
       </c>
@@ -1058,29 +2150,31 @@
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
-      <c r="L4" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="M4" s="31"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="31" t="s">
+        <v>48</v>
+      </c>
       <c r="N4" s="31"/>
-      <c r="O4" s="21" t="s">
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
       <c r="R4" s="21"/>
       <c r="S4" s="21"/>
       <c r="T4" s="21"/>
-    </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="U4" s="21"/>
+      <c r="V4" s="21"/>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.35">
       <c r="E6" s="35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="36"/>
       <c r="G6" s="36"/>
       <c r="H6" s="37"/>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B7" s="14" t="s">
         <v>2</v>
       </c>
@@ -1088,61 +2182,70 @@
         <v>14</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E7" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="34" t="s">
+      <c r="H7" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="J7" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="L7" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="O7" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="J7" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="K7" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="L7" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="M7" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="N7" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="O7" s="19" t="s">
+      <c r="P7" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="P7" s="19" t="s">
+      <c r="R7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="Q7" s="19" t="s">
+      <c r="S7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="R7" s="19" t="s">
+      <c r="T7" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="S7" s="19" t="s">
+      <c r="U7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="T7" s="19" t="s">
+      <c r="V7" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="U7" s="28" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="W7" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="X7" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B8" s="15">
         <v>1</v>
       </c>
@@ -1150,7 +2253,7 @@
         <v>15</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" s="25">
         <v>116</v>
@@ -1164,53 +2267,59 @@
       <c r="H8" s="26">
         <v>55</v>
       </c>
-      <c r="I8" s="26">
+      <c r="I8" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="J8" s="26">
         <v>20</v>
-      </c>
-      <c r="J8" s="26">
-        <v>32</v>
       </c>
       <c r="K8" s="26">
         <v>32</v>
       </c>
-      <c r="L8" s="32">
+      <c r="L8" s="26">
+        <v>32</v>
+      </c>
+      <c r="M8" s="32">
         <v>3</v>
       </c>
-      <c r="M8" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="N8" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="O8" s="23">
-        <f>IFERROR(Q8/(Q8+R8),"-")</f>
+      <c r="N8" s="32">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O8" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="P8" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q8" s="23">
+        <f>IFERROR(S8/(S8+T8),"-")</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="P8" s="23">
-        <f>IFERROR(Q8/(Q8+T8),"-")</f>
+      <c r="R8" s="23">
+        <f>IFERROR(S8/(S8+V8),"-")</f>
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="Q8" s="22">
+      <c r="S8" s="22">
         <f>SUMIFS(Test_Logs!F$9:F$113,Test_Logs!$B$9:$B$113,$B8)</f>
         <v>1</v>
       </c>
-      <c r="R8" s="22">
+      <c r="T8" s="22">
         <f>SUMIFS(Test_Logs!G$9:G$113,Test_Logs!$B$9:$B$113,$B8)</f>
         <v>11</v>
       </c>
-      <c r="S8" s="22">
+      <c r="U8" s="22">
         <f>SUMIFS(Test_Logs!H$9:H$113,Test_Logs!$B$9:$B$113,$B8)</f>
         <v>7</v>
       </c>
-      <c r="T8" s="22">
+      <c r="V8" s="22">
         <f>SUMIFS(Test_Logs!I$9:I$113,Test_Logs!$B$9:$B$113,$B8)</f>
         <v>10</v>
       </c>
-      <c r="U8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="W8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B9" s="15">
         <f>B8+1</f>
         <v>2</v>
@@ -1219,7 +2328,7 @@
         <v>16</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" s="25">
         <v>116</v>
@@ -1233,62 +2342,68 @@
       <c r="H9" s="26">
         <v>55</v>
       </c>
-      <c r="I9" s="26">
+      <c r="I9" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="J9" s="26">
         <v>20</v>
       </c>
-      <c r="J9" s="26">
+      <c r="K9" s="26">
         <v>48</v>
       </c>
-      <c r="K9" s="26">
+      <c r="L9" s="26">
         <v>24</v>
       </c>
-      <c r="L9" s="32">
+      <c r="M9" s="32">
         <v>3</v>
       </c>
-      <c r="M9" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="N9" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="O9" s="23" t="str">
-        <f t="shared" ref="O9:O13" si="0">IFERROR(Q9/(Q9+R9),"-")</f>
+      <c r="N9" s="32">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O9" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="P9" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q9" s="23" t="str">
+        <f t="shared" ref="Q9:Q13" si="0">IFERROR(S9/(S9+T9),"-")</f>
         <v>-</v>
       </c>
-      <c r="P9" s="23">
-        <f t="shared" ref="P9:P13" si="1">IFERROR(Q9/(Q9+T9),"-")</f>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="22">
+      <c r="R9" s="23">
+        <f t="shared" ref="R9:R13" si="1">IFERROR(S9/(S9+V9),"-")</f>
+        <v>0</v>
+      </c>
+      <c r="S9" s="22">
         <f>SUMIFS(Test_Logs!F$9:F$113,Test_Logs!$B$9:$B$113,$B9)</f>
         <v>0</v>
       </c>
-      <c r="R9" s="22">
+      <c r="T9" s="22">
         <f>SUMIFS(Test_Logs!G$9:G$113,Test_Logs!$B$9:$B$113,$B9)</f>
         <v>0</v>
       </c>
-      <c r="S9" s="22">
+      <c r="U9" s="22">
         <f>SUMIFS(Test_Logs!H$9:H$113,Test_Logs!$B$9:$B$113,$B9)</f>
         <v>8</v>
       </c>
-      <c r="T9" s="22">
+      <c r="V9" s="22">
         <f>SUMIFS(Test_Logs!I$9:I$113,Test_Logs!$B$9:$B$113,$B9)</f>
         <v>11</v>
       </c>
-      <c r="U9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="X9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B10" s="15">
         <f t="shared" ref="B10:B19" si="2">B9+1</f>
         <v>3</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E10" s="25">
         <v>44</v>
@@ -1302,62 +2417,68 @@
       <c r="H10" s="26">
         <v>44</v>
       </c>
-      <c r="I10" s="26">
+      <c r="I10" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="J10" s="26">
         <v>20</v>
       </c>
-      <c r="J10" s="26">
+      <c r="K10" s="26">
         <v>24</v>
       </c>
-      <c r="K10" s="26">
+      <c r="L10" s="26">
         <v>48</v>
       </c>
-      <c r="L10" s="32">
+      <c r="M10" s="32">
         <v>3</v>
       </c>
-      <c r="M10" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="N10" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="O10" s="23">
+      <c r="N10" s="32">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O10" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="P10" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q10" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P10" s="23">
+      <c r="R10" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q10" s="22">
+      <c r="S10" s="22">
         <f>SUMIFS(Test_Logs!F$9:F$113,Test_Logs!$B$9:$B$113,$B10)</f>
         <v>0</v>
       </c>
-      <c r="R10" s="22">
+      <c r="T10" s="22">
         <f>SUMIFS(Test_Logs!G$9:G$113,Test_Logs!$B$9:$B$113,$B10)</f>
         <v>1</v>
       </c>
-      <c r="S10" s="22">
+      <c r="U10" s="22">
         <f>SUMIFS(Test_Logs!H$9:H$113,Test_Logs!$B$9:$B$113,$B10)</f>
         <v>7</v>
       </c>
-      <c r="T10" s="22">
+      <c r="V10" s="22">
         <f>SUMIFS(Test_Logs!I$9:I$113,Test_Logs!$B$9:$B$113,$B10)</f>
         <v>11</v>
       </c>
-      <c r="U10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="X10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B11" s="15">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" s="25">
         <v>209</v>
@@ -1371,167 +2492,281 @@
       <c r="H11" s="26">
         <v>470</v>
       </c>
-      <c r="I11" s="26">
-        <v>20</v>
+      <c r="I11" s="26" t="s">
+        <v>62</v>
       </c>
       <c r="J11" s="26">
+        <v>6</v>
+      </c>
+      <c r="K11" s="26">
         <v>24</v>
       </c>
-      <c r="K11" s="26">
+      <c r="L11" s="26">
         <v>46</v>
       </c>
-      <c r="L11" s="32">
+      <c r="M11" s="32">
         <v>3</v>
       </c>
-      <c r="M11" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="N11" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="O11" s="23">
+      <c r="N11" s="32">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O11" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="P11" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q11" s="23">
         <f t="shared" si="0"/>
         <v>0.17647058823529413</v>
       </c>
-      <c r="P11" s="23">
+      <c r="R11" s="23">
         <f t="shared" si="1"/>
         <v>0.27272727272727271</v>
       </c>
-      <c r="Q11" s="22">
+      <c r="S11" s="22">
         <f>SUMIFS(Test_Logs!F$9:F$113,Test_Logs!$B$9:$B$113,$B11)</f>
         <v>3</v>
       </c>
-      <c r="R11" s="22">
+      <c r="T11" s="22">
         <f>SUMIFS(Test_Logs!G$9:G$113,Test_Logs!$B$9:$B$113,$B11)</f>
         <v>14</v>
       </c>
-      <c r="S11" s="22">
+      <c r="U11" s="22">
         <f>SUMIFS(Test_Logs!H$9:H$113,Test_Logs!$B$9:$B$113,$B11)</f>
         <v>5</v>
       </c>
-      <c r="T11" s="22">
+      <c r="V11" s="22">
         <f>SUMIFS(Test_Logs!I$9:I$113,Test_Logs!$B$9:$B$113,$B11)</f>
         <v>8</v>
       </c>
-      <c r="U11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="X11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B12" s="15">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="32"/>
-      <c r="O12" s="23" t="str">
+      <c r="C12" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="25">
+        <v>244</v>
+      </c>
+      <c r="F12" s="25">
+        <v>255</v>
+      </c>
+      <c r="G12" s="25">
+        <v>1464</v>
+      </c>
+      <c r="H12" s="26">
+        <v>1530</v>
+      </c>
+      <c r="I12" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="J12" s="26">
+        <v>8</v>
+      </c>
+      <c r="K12" s="26">
+        <v>24</v>
+      </c>
+      <c r="L12" s="26">
+        <v>46</v>
+      </c>
+      <c r="M12" s="32">
+        <v>3</v>
+      </c>
+      <c r="N12" s="32">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O12" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="P12" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q12" s="23">
         <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="P12" s="23" t="str">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="R12" s="23">
         <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="Q12" s="22">
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="S12" s="22">
         <f>SUMIFS(Test_Logs!F$9:F$113,Test_Logs!$B$9:$B$113,$B12)</f>
-        <v>0</v>
-      </c>
-      <c r="R12" s="22">
+        <v>5</v>
+      </c>
+      <c r="T12" s="22">
         <f>SUMIFS(Test_Logs!G$9:G$113,Test_Logs!$B$9:$B$113,$B12)</f>
-        <v>0</v>
-      </c>
-      <c r="S12" s="22">
+        <v>19</v>
+      </c>
+      <c r="U12" s="22">
         <f>SUMIFS(Test_Logs!H$9:H$113,Test_Logs!$B$9:$B$113,$B12)</f>
-        <v>0</v>
-      </c>
-      <c r="T12" s="22">
+        <v>3</v>
+      </c>
+      <c r="V12" s="22">
         <f>SUMIFS(Test_Logs!I$9:I$113,Test_Logs!$B$9:$B$113,$B12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="W12" t="s">
+        <v>58</v>
+      </c>
+      <c r="X12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B13" s="15">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="23" t="str">
+      <c r="C13" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="25">
+        <v>244</v>
+      </c>
+      <c r="F13" s="25">
+        <v>255</v>
+      </c>
+      <c r="G13" s="25">
+        <v>1464</v>
+      </c>
+      <c r="H13" s="26">
+        <v>1530</v>
+      </c>
+      <c r="I13" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" s="26">
+        <v>8</v>
+      </c>
+      <c r="K13" s="26">
+        <v>24</v>
+      </c>
+      <c r="L13" s="26">
+        <v>46</v>
+      </c>
+      <c r="M13" s="32">
+        <v>3</v>
+      </c>
+      <c r="N13" s="32">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O13" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="P13" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q13" s="23">
         <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="P13" s="23" t="str">
+        <v>0.28125</v>
+      </c>
+      <c r="R13" s="23">
         <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="Q13" s="22">
+        <v>0.81818181818181823</v>
+      </c>
+      <c r="S13" s="22">
         <f>SUMIFS(Test_Logs!F$9:F$113,Test_Logs!$B$9:$B$113,$B13)</f>
-        <v>0</v>
-      </c>
-      <c r="R13" s="22">
+        <v>9</v>
+      </c>
+      <c r="T13" s="22">
         <f>SUMIFS(Test_Logs!G$9:G$113,Test_Logs!$B$9:$B$113,$B13)</f>
-        <v>0</v>
-      </c>
-      <c r="S13" s="22">
+        <v>23</v>
+      </c>
+      <c r="U13" s="22">
         <f>SUMIFS(Test_Logs!H$9:H$113,Test_Logs!$B$9:$B$113,$B13)</f>
-        <v>0</v>
-      </c>
-      <c r="T13" s="22">
+        <v>3</v>
+      </c>
+      <c r="V13" s="22">
         <f>SUMIFS(Test_Logs!I$9:I$113,Test_Logs!$B$9:$B$113,$B13)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B14" s="15">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="32"/>
-      <c r="O14" s="23" t="str">
-        <f t="shared" ref="O14:O19" si="3">IFERROR(Q14/(Q14+R14),"-")</f>
-        <v>-</v>
-      </c>
-      <c r="P14" s="23" t="str">
-        <f t="shared" ref="P14:P19" si="4">IFERROR(Q14/(Q14+T14),"-")</f>
-        <v>-</v>
-      </c>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="22"/>
-      <c r="S14" s="22"/>
-      <c r="T14" s="22"/>
-    </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="C14" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="25">
+        <v>244</v>
+      </c>
+      <c r="F14" s="25">
+        <v>255</v>
+      </c>
+      <c r="G14" s="25">
+        <v>1464</v>
+      </c>
+      <c r="H14" s="26">
+        <v>1530</v>
+      </c>
+      <c r="I14" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" s="26">
+        <v>10</v>
+      </c>
+      <c r="K14" s="26">
+        <v>24</v>
+      </c>
+      <c r="L14" s="26">
+        <v>46</v>
+      </c>
+      <c r="M14" s="32">
+        <v>13</v>
+      </c>
+      <c r="N14" s="32">
+        <v>1.2</v>
+      </c>
+      <c r="O14" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="P14" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q14" s="23">
+        <f t="shared" ref="Q14:Q19" si="3">IFERROR(S14/(S14+T14),"-")</f>
+        <v>0.8</v>
+      </c>
+      <c r="R14" s="23">
+        <f t="shared" ref="R14:R19" si="4">IFERROR(S14/(S14+V14),"-")</f>
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="S14" s="22">
+        <f>SUMIFS(Test_Logs!F$9:F$113,Test_Logs!$B$9:$B$113,$B14)</f>
+        <v>8</v>
+      </c>
+      <c r="T14" s="22">
+        <f>SUMIFS(Test_Logs!G$9:G$113,Test_Logs!$B$9:$B$113,$B14)</f>
+        <v>2</v>
+      </c>
+      <c r="U14" s="22">
+        <f>SUMIFS(Test_Logs!H$9:H$113,Test_Logs!$B$9:$B$113,$B14)</f>
+        <v>7</v>
+      </c>
+      <c r="V14" s="22">
+        <f>SUMIFS(Test_Logs!I$9:I$113,Test_Logs!$B$9:$B$113,$B14)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B15" s="15">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -1545,23 +2780,37 @@
       <c r="I15" s="26"/>
       <c r="J15" s="26"/>
       <c r="K15" s="26"/>
-      <c r="L15" s="32"/>
+      <c r="L15" s="26"/>
       <c r="M15" s="32"/>
       <c r="N15" s="32"/>
-      <c r="O15" s="23" t="str">
+      <c r="O15" s="32"/>
+      <c r="P15" s="32"/>
+      <c r="Q15" s="23" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="P15" s="23" t="str">
+      <c r="R15" s="23" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="22"/>
-      <c r="S15" s="22"/>
-      <c r="T15" s="22"/>
-    </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="S15" s="22">
+        <f>SUMIFS(Test_Logs!F$9:F$113,Test_Logs!$B$9:$B$113,$B15)</f>
+        <v>0</v>
+      </c>
+      <c r="T15" s="22">
+        <f>SUMIFS(Test_Logs!G$9:G$113,Test_Logs!$B$9:$B$113,$B15)</f>
+        <v>0</v>
+      </c>
+      <c r="U15" s="22">
+        <f>SUMIFS(Test_Logs!H$9:H$113,Test_Logs!$B$9:$B$113,$B15)</f>
+        <v>0</v>
+      </c>
+      <c r="V15" s="22">
+        <f>SUMIFS(Test_Logs!I$9:I$113,Test_Logs!$B$9:$B$113,$B15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B16" s="15">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -1575,23 +2824,37 @@
       <c r="I16" s="26"/>
       <c r="J16" s="26"/>
       <c r="K16" s="26"/>
-      <c r="L16" s="32"/>
+      <c r="L16" s="26"/>
       <c r="M16" s="32"/>
       <c r="N16" s="32"/>
-      <c r="O16" s="23" t="str">
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="23" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="P16" s="23" t="str">
+      <c r="R16" s="23" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="22"/>
-      <c r="S16" s="22"/>
-      <c r="T16" s="22"/>
-    </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="S16" s="22">
+        <f>SUMIFS(Test_Logs!F$9:F$113,Test_Logs!$B$9:$B$113,$B16)</f>
+        <v>0</v>
+      </c>
+      <c r="T16" s="22">
+        <f>SUMIFS(Test_Logs!G$9:G$113,Test_Logs!$B$9:$B$113,$B16)</f>
+        <v>0</v>
+      </c>
+      <c r="U16" s="22">
+        <f>SUMIFS(Test_Logs!H$9:H$113,Test_Logs!$B$9:$B$113,$B16)</f>
+        <v>0</v>
+      </c>
+      <c r="V16" s="22">
+        <f>SUMIFS(Test_Logs!I$9:I$113,Test_Logs!$B$9:$B$113,$B16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B17" s="15">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -1605,23 +2868,37 @@
       <c r="I17" s="26"/>
       <c r="J17" s="26"/>
       <c r="K17" s="26"/>
-      <c r="L17" s="32"/>
+      <c r="L17" s="26"/>
       <c r="M17" s="32"/>
       <c r="N17" s="32"/>
-      <c r="O17" s="23" t="str">
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="23" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="P17" s="23" t="str">
+      <c r="R17" s="23" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="22"/>
-      <c r="S17" s="22"/>
-      <c r="T17" s="22"/>
-    </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="S17" s="22">
+        <f>SUMIFS(Test_Logs!F$9:F$113,Test_Logs!$B$9:$B$113,$B17)</f>
+        <v>0</v>
+      </c>
+      <c r="T17" s="22">
+        <f>SUMIFS(Test_Logs!G$9:G$113,Test_Logs!$B$9:$B$113,$B17)</f>
+        <v>0</v>
+      </c>
+      <c r="U17" s="22">
+        <f>SUMIFS(Test_Logs!H$9:H$113,Test_Logs!$B$9:$B$113,$B17)</f>
+        <v>0</v>
+      </c>
+      <c r="V17" s="22">
+        <f>SUMIFS(Test_Logs!I$9:I$113,Test_Logs!$B$9:$B$113,$B17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B18" s="15">
         <f t="shared" si="2"/>
         <v>11</v>
@@ -1635,35 +2912,37 @@
       <c r="I18" s="26"/>
       <c r="J18" s="26"/>
       <c r="K18" s="26"/>
-      <c r="L18" s="32"/>
+      <c r="L18" s="26"/>
       <c r="M18" s="32"/>
       <c r="N18" s="32"/>
-      <c r="O18" s="23" t="str">
+      <c r="O18" s="32"/>
+      <c r="P18" s="32"/>
+      <c r="Q18" s="23" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="P18" s="23" t="str">
+      <c r="R18" s="23" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="Q18" s="22">
+      <c r="S18" s="22">
         <f>SUMIFS(Test_Logs!F$9:F$113,Test_Logs!$B$9:$B$113,$B18)</f>
         <v>0</v>
       </c>
-      <c r="R18" s="22">
+      <c r="T18" s="22">
         <f>SUMIFS(Test_Logs!G$9:G$113,Test_Logs!$B$9:$B$113,$B18)</f>
         <v>0</v>
       </c>
-      <c r="S18" s="22">
+      <c r="U18" s="22">
         <f>SUMIFS(Test_Logs!H$9:H$113,Test_Logs!$B$9:$B$113,$B18)</f>
         <v>0</v>
       </c>
-      <c r="T18" s="22">
+      <c r="V18" s="22">
         <f>SUMIFS(Test_Logs!I$9:I$113,Test_Logs!$B$9:$B$113,$B18)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B19" s="15">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -1677,33 +2956,53 @@
       <c r="I19" s="26"/>
       <c r="J19" s="26"/>
       <c r="K19" s="26"/>
-      <c r="L19" s="32"/>
+      <c r="L19" s="26"/>
       <c r="M19" s="32"/>
       <c r="N19" s="32"/>
-      <c r="O19" s="23" t="str">
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="23" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="P19" s="23" t="str">
+      <c r="R19" s="23" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="Q19" s="22">
+      <c r="S19" s="22">
         <f>SUMIFS(Test_Logs!F$9:F$113,Test_Logs!$B$9:$B$113,$B19)</f>
         <v>0</v>
       </c>
-      <c r="R19" s="22">
+      <c r="T19" s="22">
         <f>SUMIFS(Test_Logs!G$9:G$113,Test_Logs!$B$9:$B$113,$B19)</f>
         <v>0</v>
       </c>
-      <c r="S19" s="22">
+      <c r="U19" s="22">
         <f>SUMIFS(Test_Logs!H$9:H$113,Test_Logs!$B$9:$B$113,$B19)</f>
         <v>0</v>
       </c>
-      <c r="T19" s="22">
+      <c r="V19" s="22">
         <f>SUMIFS(Test_Logs!I$9:I$113,Test_Logs!$B$9:$B$113,$B19)</f>
         <v>0</v>
       </c>
+    </row>
+    <row r="26" spans="2:22" ht="17" x14ac:dyDescent="0.4">
+      <c r="B26" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="57"/>
+      <c r="K26" s="57"/>
+      <c r="L26" s="57"/>
+      <c r="M26" s="57"/>
+      <c r="N26" s="57"/>
+      <c r="O26" s="57"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1716,7 +3015,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D67C8FC6-D7B6-46A9-9A06-D0E7B7D96350}">
   <dimension ref="B1:Y147"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane xSplit="1" ySplit="8" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1836,10 +3140,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="10">
         <v>3</v>
@@ -1884,10 +3188,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="10">
         <v>2</v>
@@ -1932,10 +3236,10 @@
         <v>1</v>
       </c>
       <c r="C11" s="52" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="10">
         <v>2</v>
@@ -1980,10 +3284,10 @@
         <v>1</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="10">
         <v>2</v>
@@ -2028,10 +3332,10 @@
         <v>1</v>
       </c>
       <c r="C13" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" s="10">
         <v>2</v>
@@ -2057,7 +3361,7 @@
         <v>0.5</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
@@ -2078,10 +3382,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="52" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E14" s="10">
         <v>0</v>
@@ -2126,10 +3430,10 @@
         <v>1</v>
       </c>
       <c r="C15" s="52" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E15" s="10">
         <v>0</v>
@@ -2174,10 +3478,10 @@
         <v>1</v>
       </c>
       <c r="C16" s="52" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E16" s="10">
         <v>0</v>
@@ -2222,10 +3526,10 @@
         <v>1</v>
       </c>
       <c r="C17" s="52" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E17" s="10">
         <v>0</v>
@@ -2270,10 +3574,10 @@
         <v>1</v>
       </c>
       <c r="C18" s="54" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18" s="46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E18" s="47">
         <v>0</v>
@@ -2318,10 +3622,10 @@
         <v>2</v>
       </c>
       <c r="C19" s="56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" s="40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E19" s="41">
         <v>3</v>
@@ -2366,10 +3670,10 @@
         <v>2</v>
       </c>
       <c r="C20" s="52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E20" s="10">
         <v>2</v>
@@ -2414,10 +3718,10 @@
         <v>2</v>
       </c>
       <c r="C21" s="52" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E21" s="10">
         <v>2</v>
@@ -2462,10 +3766,10 @@
         <v>2</v>
       </c>
       <c r="C22" s="52" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E22" s="10">
         <v>2</v>
@@ -2510,10 +3814,10 @@
         <v>2</v>
       </c>
       <c r="C23" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E23" s="10">
         <v>2</v>
@@ -2558,10 +3862,10 @@
         <v>2</v>
       </c>
       <c r="C24" s="52" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E24" s="10">
         <v>0</v>
@@ -2606,10 +3910,10 @@
         <v>2</v>
       </c>
       <c r="C25" s="52" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E25" s="10">
         <v>0</v>
@@ -2654,10 +3958,10 @@
         <v>2</v>
       </c>
       <c r="C26" s="52" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E26" s="10">
         <v>0</v>
@@ -2702,10 +4006,10 @@
         <v>2</v>
       </c>
       <c r="C27" s="52" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E27" s="10">
         <v>0</v>
@@ -2750,10 +4054,10 @@
         <v>2</v>
       </c>
       <c r="C28" s="54" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D28" s="46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E28" s="47">
         <v>0</v>
@@ -2798,10 +4102,10 @@
         <v>3</v>
       </c>
       <c r="C29" s="56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E29" s="41">
         <v>3</v>
@@ -2846,10 +4150,10 @@
         <v>3</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D30" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E30" s="10">
         <v>2</v>
@@ -2894,10 +4198,10 @@
         <v>3</v>
       </c>
       <c r="C31" s="52" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E31" s="10">
         <v>2</v>
@@ -2942,10 +4246,10 @@
         <v>3</v>
       </c>
       <c r="C32" s="52" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D32" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E32" s="10">
         <v>2</v>
@@ -2990,10 +4294,10 @@
         <v>3</v>
       </c>
       <c r="C33" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D33" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E33" s="10">
         <v>2</v>
@@ -3038,10 +4342,10 @@
         <v>3</v>
       </c>
       <c r="C34" s="52" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D34" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E34" s="10">
         <v>0</v>
@@ -3086,10 +4390,10 @@
         <v>3</v>
       </c>
       <c r="C35" s="52" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D35" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E35" s="10">
         <v>0</v>
@@ -3134,10 +4438,10 @@
         <v>3</v>
       </c>
       <c r="C36" s="52" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E36" s="10">
         <v>0</v>
@@ -3182,10 +4486,10 @@
         <v>3</v>
       </c>
       <c r="C37" s="52" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E37" s="10">
         <v>0</v>
@@ -3230,10 +4534,10 @@
         <v>3</v>
       </c>
       <c r="C38" s="54" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D38" s="46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E38" s="47">
         <v>0</v>
@@ -3278,10 +4582,10 @@
         <v>4</v>
       </c>
       <c r="C39" s="56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D39" s="40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E39" s="41">
         <v>3</v>
@@ -3326,10 +4630,10 @@
         <v>4</v>
       </c>
       <c r="C40" s="52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E40" s="10">
         <v>2</v>
@@ -3374,10 +4678,10 @@
         <v>4</v>
       </c>
       <c r="C41" s="52" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E41" s="10">
         <v>2</v>
@@ -3422,10 +4726,10 @@
         <v>4</v>
       </c>
       <c r="C42" s="52" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E42" s="10">
         <v>2</v>
@@ -3470,10 +4774,10 @@
         <v>4</v>
       </c>
       <c r="C43" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E43" s="10">
         <v>2</v>
@@ -3499,7 +4803,7 @@
         <v>0.5</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
@@ -3520,10 +4824,10 @@
         <v>4</v>
       </c>
       <c r="C44" s="52" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E44" s="10">
         <v>0</v>
@@ -3568,10 +4872,10 @@
         <v>4</v>
       </c>
       <c r="C45" s="52" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E45" s="10">
         <v>0</v>
@@ -3616,10 +4920,10 @@
         <v>4</v>
       </c>
       <c r="C46" s="52" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E46" s="10">
         <v>0</v>
@@ -3637,11 +4941,11 @@
         <v>0</v>
       </c>
       <c r="J46" s="38">
-        <f t="shared" ref="J46:J48" si="6">IFERROR(F46/(F46+G46),0)</f>
+        <f t="shared" ref="J46:J55" si="6">IFERROR(F46/(F46+G46),0)</f>
         <v>0</v>
       </c>
       <c r="K46" s="38">
-        <f t="shared" ref="K46:K48" si="7">IFERROR(F46/(F46+I46),0)</f>
+        <f t="shared" ref="K46:K55" si="7">IFERROR(F46/(F46+I46),0)</f>
         <v>0</v>
       </c>
       <c r="L46" s="8"/>
@@ -3664,10 +4968,10 @@
         <v>4</v>
       </c>
       <c r="C47" s="52" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D47" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E47" s="10">
         <v>0</v>
@@ -3708,14 +5012,14 @@
       <c r="Y47" s="3"/>
     </row>
     <row r="48" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B48" s="55">
+      <c r="B48" s="53">
         <v>4</v>
       </c>
       <c r="C48" s="54" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D48" s="46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E48" s="47">
         <v>0</v>
@@ -3756,23 +5060,39 @@
       <c r="Y48" s="3"/>
     </row>
     <row r="49" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B49" s="18"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="27"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="16"/>
-      <c r="G49" s="16"/>
-      <c r="H49" s="16"/>
-      <c r="I49" s="17"/>
-      <c r="J49" s="38">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K49" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L49" s="8"/>
+      <c r="B49" s="55">
+        <v>5</v>
+      </c>
+      <c r="C49" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="E49" s="41">
+        <v>3</v>
+      </c>
+      <c r="F49" s="42">
+        <v>3</v>
+      </c>
+      <c r="G49" s="42">
+        <v>0</v>
+      </c>
+      <c r="H49" s="42">
+        <v>3</v>
+      </c>
+      <c r="I49" s="43">
+        <v>0</v>
+      </c>
+      <c r="J49" s="44">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="K49" s="44">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="L49" s="39"/>
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
       <c r="O49" s="3"/>
@@ -3788,20 +5108,36 @@
       <c r="Y49" s="3"/>
     </row>
     <row r="50" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B50" s="18"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="16"/>
-      <c r="H50" s="16"/>
-      <c r="I50" s="17"/>
+      <c r="B50" s="55">
+        <v>5</v>
+      </c>
+      <c r="C50" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E50" s="10">
+        <v>2</v>
+      </c>
+      <c r="F50" s="16">
+        <v>0</v>
+      </c>
+      <c r="G50" s="16">
+        <v>0</v>
+      </c>
+      <c r="H50" s="16">
+        <v>0</v>
+      </c>
+      <c r="I50" s="17">
+        <v>2</v>
+      </c>
       <c r="J50" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K50" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L50" s="8"/>
@@ -3820,20 +5156,36 @@
       <c r="Y50" s="3"/>
     </row>
     <row r="51" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B51" s="18"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="27"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="16"/>
-      <c r="G51" s="16"/>
-      <c r="H51" s="16"/>
-      <c r="I51" s="17"/>
+      <c r="B51" s="55">
+        <v>5</v>
+      </c>
+      <c r="C51" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="D51" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E51" s="10">
+        <v>2</v>
+      </c>
+      <c r="F51" s="16">
+        <v>0</v>
+      </c>
+      <c r="G51" s="16">
+        <v>0</v>
+      </c>
+      <c r="H51" s="16">
+        <v>0</v>
+      </c>
+      <c r="I51" s="17">
+        <v>2</v>
+      </c>
       <c r="J51" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K51" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L51" s="8"/>
@@ -3852,20 +5204,36 @@
       <c r="Y51" s="3"/>
     </row>
     <row r="52" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B52" s="18"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="16"/>
-      <c r="G52" s="16"/>
-      <c r="H52" s="16"/>
-      <c r="I52" s="17"/>
+      <c r="B52" s="55">
+        <v>5</v>
+      </c>
+      <c r="C52" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="D52" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E52" s="10">
+        <v>2</v>
+      </c>
+      <c r="F52" s="16">
+        <v>0</v>
+      </c>
+      <c r="G52" s="16">
+        <v>0</v>
+      </c>
+      <c r="H52" s="16">
+        <v>0</v>
+      </c>
+      <c r="I52" s="17">
+        <v>2</v>
+      </c>
       <c r="J52" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K52" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L52" s="8"/>
@@ -3884,23 +5252,41 @@
       <c r="Y52" s="3"/>
     </row>
     <row r="53" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B53" s="18"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="27"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="16"/>
-      <c r="G53" s="16"/>
-      <c r="H53" s="16"/>
-      <c r="I53" s="17"/>
+      <c r="B53" s="55">
+        <v>5</v>
+      </c>
+      <c r="C53" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D53" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E53" s="10">
+        <v>2</v>
+      </c>
+      <c r="F53" s="16">
+        <v>2</v>
+      </c>
+      <c r="G53" s="16">
+        <v>2</v>
+      </c>
+      <c r="H53" s="16">
+        <v>0</v>
+      </c>
+      <c r="I53" s="17">
+        <v>0</v>
+      </c>
       <c r="J53" s="38">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>0.5</v>
       </c>
       <c r="K53" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L53" s="8"/>
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="L53" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="M53" s="3"/>
       <c r="N53" s="3"/>
       <c r="O53" s="3"/>
@@ -3916,20 +5302,36 @@
       <c r="Y53" s="3"/>
     </row>
     <row r="54" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B54" s="18"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="16"/>
-      <c r="H54" s="16"/>
-      <c r="I54" s="17"/>
+      <c r="B54" s="55">
+        <v>5</v>
+      </c>
+      <c r="C54" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="D54" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E54" s="10">
+        <v>0</v>
+      </c>
+      <c r="F54" s="16">
+        <v>0</v>
+      </c>
+      <c r="G54" s="16">
+        <v>10</v>
+      </c>
+      <c r="H54" s="16">
+        <v>0</v>
+      </c>
+      <c r="I54" s="17">
+        <v>0</v>
+      </c>
       <c r="J54" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K54" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L54" s="8"/>
@@ -3948,20 +5350,36 @@
       <c r="Y54" s="3"/>
     </row>
     <row r="55" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B55" s="18"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="16"/>
-      <c r="G55" s="16"/>
-      <c r="H55" s="16"/>
-      <c r="I55" s="17"/>
+      <c r="B55" s="55">
+        <v>5</v>
+      </c>
+      <c r="C55" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="D55" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E55" s="10">
+        <v>0</v>
+      </c>
+      <c r="F55" s="16">
+        <v>0</v>
+      </c>
+      <c r="G55" s="16">
+        <v>2</v>
+      </c>
+      <c r="H55" s="16">
+        <v>0</v>
+      </c>
+      <c r="I55" s="17">
+        <v>0</v>
+      </c>
       <c r="J55" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K55" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L55" s="8"/>
@@ -3980,20 +5398,36 @@
       <c r="Y55" s="3"/>
     </row>
     <row r="56" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B56" s="18"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="27"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="16"/>
-      <c r="H56" s="16"/>
-      <c r="I56" s="17"/>
+      <c r="B56" s="55">
+        <v>5</v>
+      </c>
+      <c r="C56" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="D56" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E56" s="10">
+        <v>0</v>
+      </c>
+      <c r="F56" s="16">
+        <v>0</v>
+      </c>
+      <c r="G56" s="16">
+        <v>2</v>
+      </c>
+      <c r="H56" s="16">
+        <v>0</v>
+      </c>
+      <c r="I56" s="17">
+        <v>0</v>
+      </c>
       <c r="J56" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="J56:J58" si="8">IFERROR(F56/(F56+G56),0)</f>
         <v>0</v>
       </c>
       <c r="K56" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="K56:K58" si="9">IFERROR(F56/(F56+I56),0)</f>
         <v>0</v>
       </c>
       <c r="L56" s="8"/>
@@ -4012,20 +5446,36 @@
       <c r="Y56" s="3"/>
     </row>
     <row r="57" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B57" s="18"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="27"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="16"/>
-      <c r="G57" s="16"/>
-      <c r="H57" s="16"/>
-      <c r="I57" s="17"/>
+      <c r="B57" s="55">
+        <v>5</v>
+      </c>
+      <c r="C57" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="D57" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E57" s="10">
+        <v>0</v>
+      </c>
+      <c r="F57" s="16">
+        <v>0</v>
+      </c>
+      <c r="G57" s="16">
+        <v>2</v>
+      </c>
+      <c r="H57" s="16">
+        <v>0</v>
+      </c>
+      <c r="I57" s="17">
+        <v>0</v>
+      </c>
       <c r="J57" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K57" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="L57" s="8"/>
@@ -4044,23 +5494,39 @@
       <c r="Y57" s="3"/>
     </row>
     <row r="58" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B58" s="18"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="27"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="16"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="17"/>
-      <c r="J58" s="38">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K58" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L58" s="8"/>
+      <c r="B58" s="53">
+        <v>5</v>
+      </c>
+      <c r="C58" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="D58" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="E58" s="47">
+        <v>0</v>
+      </c>
+      <c r="F58" s="48">
+        <v>0</v>
+      </c>
+      <c r="G58" s="48">
+        <v>1</v>
+      </c>
+      <c r="H58" s="48">
+        <v>0</v>
+      </c>
+      <c r="I58" s="49">
+        <v>0</v>
+      </c>
+      <c r="J58" s="50">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K58" s="50">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L58" s="45"/>
       <c r="M58" s="3"/>
       <c r="N58" s="3"/>
       <c r="O58" s="3"/>
@@ -4076,21 +5542,37 @@
       <c r="Y58" s="3"/>
     </row>
     <row r="59" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B59" s="18"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="27"/>
-      <c r="E59" s="10"/>
-      <c r="F59" s="16"/>
-      <c r="G59" s="16"/>
-      <c r="H59" s="16"/>
-      <c r="I59" s="17"/>
+      <c r="B59" s="55">
+        <v>6</v>
+      </c>
+      <c r="C59" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="D59" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="E59" s="41">
+        <v>3</v>
+      </c>
+      <c r="F59" s="42">
+        <v>3</v>
+      </c>
+      <c r="G59" s="42">
+        <v>0</v>
+      </c>
+      <c r="H59" s="42">
+        <v>3</v>
+      </c>
+      <c r="I59" s="43">
+        <v>0</v>
+      </c>
       <c r="J59" s="38">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K59" s="38">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L59" s="8"/>
       <c r="M59" s="3"/>
@@ -4108,14 +5590,30 @@
       <c r="Y59" s="3"/>
     </row>
     <row r="60" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B60" s="18"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="27"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="16"/>
-      <c r="G60" s="16"/>
-      <c r="H60" s="16"/>
-      <c r="I60" s="17"/>
+      <c r="B60" s="55">
+        <v>6</v>
+      </c>
+      <c r="C60" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E60" s="10">
+        <v>2</v>
+      </c>
+      <c r="F60" s="16">
+        <v>0</v>
+      </c>
+      <c r="G60" s="16">
+        <v>0</v>
+      </c>
+      <c r="H60" s="16">
+        <v>0</v>
+      </c>
+      <c r="I60" s="17">
+        <v>2</v>
+      </c>
       <c r="J60" s="38">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4140,21 +5638,37 @@
       <c r="Y60" s="3"/>
     </row>
     <row r="61" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B61" s="18"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="27"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="16"/>
-      <c r="G61" s="16"/>
-      <c r="H61" s="16"/>
-      <c r="I61" s="17"/>
+      <c r="B61" s="55">
+        <v>6</v>
+      </c>
+      <c r="C61" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="D61" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E61" s="10">
+        <v>2</v>
+      </c>
+      <c r="F61" s="16">
+        <v>2</v>
+      </c>
+      <c r="G61" s="16">
+        <v>2</v>
+      </c>
+      <c r="H61" s="16">
+        <v>0</v>
+      </c>
+      <c r="I61" s="17">
+        <v>0</v>
+      </c>
       <c r="J61" s="38">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K61" s="38">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L61" s="8"/>
       <c r="M61" s="3"/>
@@ -4172,21 +5686,37 @@
       <c r="Y61" s="3"/>
     </row>
     <row r="62" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B62" s="18"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="27"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="16"/>
-      <c r="G62" s="16"/>
-      <c r="H62" s="16"/>
-      <c r="I62" s="17"/>
+      <c r="B62" s="55">
+        <v>6</v>
+      </c>
+      <c r="C62" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="D62" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E62" s="10">
+        <v>2</v>
+      </c>
+      <c r="F62" s="16">
+        <v>2</v>
+      </c>
+      <c r="G62" s="16">
+        <v>2</v>
+      </c>
+      <c r="H62" s="16">
+        <v>0</v>
+      </c>
+      <c r="I62" s="17">
+        <v>0</v>
+      </c>
       <c r="J62" s="38">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K62" s="38">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L62" s="8"/>
       <c r="M62" s="3"/>
@@ -4204,21 +5734,37 @@
       <c r="Y62" s="3"/>
     </row>
     <row r="63" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B63" s="18"/>
-      <c r="C63" s="8"/>
-      <c r="D63" s="27"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="16"/>
-      <c r="G63" s="16"/>
-      <c r="H63" s="16"/>
-      <c r="I63" s="17"/>
+      <c r="B63" s="55">
+        <v>6</v>
+      </c>
+      <c r="C63" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D63" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E63" s="10">
+        <v>2</v>
+      </c>
+      <c r="F63" s="16">
+        <v>2</v>
+      </c>
+      <c r="G63" s="16">
+        <v>2</v>
+      </c>
+      <c r="H63" s="16">
+        <v>0</v>
+      </c>
+      <c r="I63" s="17">
+        <v>0</v>
+      </c>
       <c r="J63" s="38">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K63" s="38">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L63" s="8"/>
       <c r="M63" s="3"/>
@@ -4236,14 +5782,30 @@
       <c r="Y63" s="3"/>
     </row>
     <row r="64" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B64" s="18"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="27"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="16"/>
-      <c r="G64" s="16"/>
-      <c r="H64" s="16"/>
-      <c r="I64" s="17"/>
+      <c r="B64" s="55">
+        <v>6</v>
+      </c>
+      <c r="C64" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="D64" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E64" s="10">
+        <v>0</v>
+      </c>
+      <c r="F64" s="16">
+        <v>0</v>
+      </c>
+      <c r="G64" s="16">
+        <v>10</v>
+      </c>
+      <c r="H64" s="16">
+        <v>0</v>
+      </c>
+      <c r="I64" s="17">
+        <v>0</v>
+      </c>
       <c r="J64" s="38">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4268,14 +5830,30 @@
       <c r="Y64" s="3"/>
     </row>
     <row r="65" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B65" s="18"/>
-      <c r="C65" s="8"/>
-      <c r="D65" s="27"/>
-      <c r="E65" s="10"/>
-      <c r="F65" s="16"/>
-      <c r="G65" s="16"/>
-      <c r="H65" s="16"/>
-      <c r="I65" s="17"/>
+      <c r="B65" s="55">
+        <v>6</v>
+      </c>
+      <c r="C65" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="D65" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E65" s="10">
+        <v>0</v>
+      </c>
+      <c r="F65" s="16">
+        <v>0</v>
+      </c>
+      <c r="G65" s="16">
+        <v>2</v>
+      </c>
+      <c r="H65" s="16">
+        <v>0</v>
+      </c>
+      <c r="I65" s="17">
+        <v>0</v>
+      </c>
       <c r="J65" s="38">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4300,14 +5878,30 @@
       <c r="Y65" s="3"/>
     </row>
     <row r="66" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B66" s="18"/>
-      <c r="C66" s="8"/>
-      <c r="D66" s="27"/>
-      <c r="E66" s="10"/>
-      <c r="F66" s="16"/>
-      <c r="G66" s="16"/>
-      <c r="H66" s="16"/>
-      <c r="I66" s="17"/>
+      <c r="B66" s="55">
+        <v>6</v>
+      </c>
+      <c r="C66" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="D66" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E66" s="10">
+        <v>0</v>
+      </c>
+      <c r="F66" s="16">
+        <v>0</v>
+      </c>
+      <c r="G66" s="16">
+        <v>2</v>
+      </c>
+      <c r="H66" s="16">
+        <v>0</v>
+      </c>
+      <c r="I66" s="17">
+        <v>0</v>
+      </c>
       <c r="J66" s="38">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4332,14 +5926,30 @@
       <c r="Y66" s="3"/>
     </row>
     <row r="67" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B67" s="18"/>
-      <c r="C67" s="8"/>
-      <c r="D67" s="27"/>
-      <c r="E67" s="10"/>
-      <c r="F67" s="16"/>
-      <c r="G67" s="16"/>
-      <c r="H67" s="16"/>
-      <c r="I67" s="17"/>
+      <c r="B67" s="55">
+        <v>6</v>
+      </c>
+      <c r="C67" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="D67" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E67" s="10">
+        <v>0</v>
+      </c>
+      <c r="F67" s="16">
+        <v>0</v>
+      </c>
+      <c r="G67" s="16">
+        <v>2</v>
+      </c>
+      <c r="H67" s="16">
+        <v>0</v>
+      </c>
+      <c r="I67" s="17">
+        <v>0</v>
+      </c>
       <c r="J67" s="38">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4364,23 +5974,39 @@
       <c r="Y67" s="3"/>
     </row>
     <row r="68" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B68" s="18"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="27"/>
-      <c r="E68" s="10"/>
-      <c r="F68" s="16"/>
-      <c r="G68" s="16"/>
-      <c r="H68" s="16"/>
-      <c r="I68" s="17"/>
-      <c r="J68" s="38">
+      <c r="B68" s="53">
+        <v>6</v>
+      </c>
+      <c r="C68" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="D68" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="E68" s="47">
+        <v>0</v>
+      </c>
+      <c r="F68" s="48">
+        <v>0</v>
+      </c>
+      <c r="G68" s="48">
+        <v>1</v>
+      </c>
+      <c r="H68" s="48">
+        <v>0</v>
+      </c>
+      <c r="I68" s="49">
+        <v>0</v>
+      </c>
+      <c r="J68" s="50">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K68" s="38">
+      <c r="K68" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="L68" s="8"/>
+      <c r="L68" s="45"/>
       <c r="M68" s="3"/>
       <c r="N68" s="3"/>
       <c r="O68" s="3"/>
@@ -4396,21 +6022,37 @@
       <c r="Y68" s="3"/>
     </row>
     <row r="69" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B69" s="18"/>
-      <c r="C69" s="8"/>
-      <c r="D69" s="27"/>
-      <c r="E69" s="10"/>
-      <c r="F69" s="16"/>
-      <c r="G69" s="16"/>
-      <c r="H69" s="16"/>
-      <c r="I69" s="17"/>
+      <c r="B69" s="55">
+        <v>7</v>
+      </c>
+      <c r="C69" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="D69" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="E69" s="41">
+        <v>3</v>
+      </c>
+      <c r="F69" s="42">
+        <v>3</v>
+      </c>
+      <c r="G69" s="42">
+        <v>0</v>
+      </c>
+      <c r="H69" s="42">
+        <v>3</v>
+      </c>
+      <c r="I69" s="43">
+        <v>0</v>
+      </c>
       <c r="J69" s="38">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" ref="J69:J78" si="10">IFERROR(F69/(F69+G69),0)</f>
+        <v>1</v>
       </c>
       <c r="K69" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" ref="K69:K78" si="11">IFERROR(F69/(F69+I69),0)</f>
+        <v>1</v>
       </c>
       <c r="L69" s="8"/>
       <c r="M69" s="3"/>
@@ -4428,21 +6070,37 @@
       <c r="Y69" s="3"/>
     </row>
     <row r="70" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B70" s="18"/>
-      <c r="C70" s="8"/>
-      <c r="D70" s="27"/>
-      <c r="E70" s="10"/>
-      <c r="F70" s="16"/>
-      <c r="G70" s="16"/>
-      <c r="H70" s="16"/>
-      <c r="I70" s="17"/>
+      <c r="B70" s="55">
+        <v>7</v>
+      </c>
+      <c r="C70" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="D70" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E70" s="10">
+        <v>2</v>
+      </c>
+      <c r="F70" s="16">
+        <v>1</v>
+      </c>
+      <c r="G70" s="16">
+        <v>0</v>
+      </c>
+      <c r="H70" s="16">
+        <v>0</v>
+      </c>
+      <c r="I70" s="17">
+        <v>1</v>
+      </c>
       <c r="J70" s="38">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>1</v>
       </c>
       <c r="K70" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>0.5</v>
       </c>
       <c r="L70" s="8"/>
       <c r="M70" s="3"/>
@@ -4460,21 +6118,37 @@
       <c r="Y70" s="3"/>
     </row>
     <row r="71" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B71" s="18"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="27"/>
-      <c r="E71" s="10"/>
-      <c r="F71" s="16"/>
-      <c r="G71" s="16"/>
-      <c r="H71" s="16"/>
-      <c r="I71" s="17"/>
+      <c r="B71" s="55">
+        <v>7</v>
+      </c>
+      <c r="C71" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="D71" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E71" s="10">
+        <v>2</v>
+      </c>
+      <c r="F71" s="16">
+        <v>2</v>
+      </c>
+      <c r="G71" s="16">
+        <v>0</v>
+      </c>
+      <c r="H71" s="16">
+        <v>0</v>
+      </c>
+      <c r="I71" s="17">
+        <v>0</v>
+      </c>
       <c r="J71" s="38">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>1</v>
       </c>
       <c r="K71" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>1</v>
       </c>
       <c r="L71" s="8"/>
       <c r="M71" s="3"/>
@@ -4492,21 +6166,37 @@
       <c r="Y71" s="3"/>
     </row>
     <row r="72" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B72" s="18"/>
-      <c r="C72" s="8"/>
-      <c r="D72" s="27"/>
-      <c r="E72" s="10"/>
-      <c r="F72" s="16"/>
-      <c r="G72" s="16"/>
-      <c r="H72" s="16"/>
-      <c r="I72" s="17"/>
+      <c r="B72" s="55">
+        <v>7</v>
+      </c>
+      <c r="C72" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="D72" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E72" s="10">
+        <v>2</v>
+      </c>
+      <c r="F72" s="16">
+        <v>1</v>
+      </c>
+      <c r="G72" s="16">
+        <v>0</v>
+      </c>
+      <c r="H72" s="16">
+        <v>0</v>
+      </c>
+      <c r="I72" s="17">
+        <v>1</v>
+      </c>
       <c r="J72" s="38">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>1</v>
       </c>
       <c r="K72" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>0.5</v>
       </c>
       <c r="L72" s="8"/>
       <c r="M72" s="3"/>
@@ -4524,21 +6214,37 @@
       <c r="Y72" s="3"/>
     </row>
     <row r="73" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B73" s="18"/>
-      <c r="C73" s="8"/>
-      <c r="D73" s="27"/>
-      <c r="E73" s="10"/>
-      <c r="F73" s="16"/>
-      <c r="G73" s="16"/>
-      <c r="H73" s="16"/>
-      <c r="I73" s="17"/>
+      <c r="B73" s="55">
+        <v>7</v>
+      </c>
+      <c r="C73" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D73" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E73" s="10">
+        <v>2</v>
+      </c>
+      <c r="F73" s="16">
+        <v>1</v>
+      </c>
+      <c r="G73" s="16">
+        <v>0</v>
+      </c>
+      <c r="H73" s="16">
+        <v>0</v>
+      </c>
+      <c r="I73" s="17">
+        <v>1</v>
+      </c>
       <c r="J73" s="38">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>1</v>
       </c>
       <c r="K73" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>0.5</v>
       </c>
       <c r="L73" s="8"/>
       <c r="M73" s="3"/>
@@ -4556,20 +6262,36 @@
       <c r="Y73" s="3"/>
     </row>
     <row r="74" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B74" s="18"/>
-      <c r="C74" s="8"/>
-      <c r="D74" s="27"/>
-      <c r="E74" s="10"/>
-      <c r="F74" s="16"/>
-      <c r="G74" s="16"/>
-      <c r="H74" s="16"/>
-      <c r="I74" s="17"/>
+      <c r="B74" s="55">
+        <v>7</v>
+      </c>
+      <c r="C74" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="D74" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E74" s="10">
+        <v>0</v>
+      </c>
+      <c r="F74" s="16">
+        <v>0</v>
+      </c>
+      <c r="G74" s="16">
+        <v>0</v>
+      </c>
+      <c r="H74" s="16">
+        <v>1</v>
+      </c>
+      <c r="I74" s="17">
+        <v>0</v>
+      </c>
       <c r="J74" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K74" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L74" s="8"/>
@@ -4588,23 +6310,41 @@
       <c r="Y74" s="3"/>
     </row>
     <row r="75" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B75" s="18"/>
-      <c r="C75" s="8"/>
-      <c r="D75" s="27"/>
-      <c r="E75" s="10"/>
-      <c r="F75" s="16"/>
-      <c r="G75" s="16"/>
-      <c r="H75" s="16"/>
-      <c r="I75" s="17"/>
+      <c r="B75" s="55">
+        <v>7</v>
+      </c>
+      <c r="C75" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="D75" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E75" s="10">
+        <v>0</v>
+      </c>
+      <c r="F75" s="16">
+        <v>0</v>
+      </c>
+      <c r="G75" s="16">
+        <v>0</v>
+      </c>
+      <c r="H75" s="16">
+        <v>1</v>
+      </c>
+      <c r="I75" s="17">
+        <v>0</v>
+      </c>
       <c r="J75" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K75" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L75" s="8"/>
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="L75" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="M75" s="3"/>
       <c r="N75" s="3"/>
       <c r="O75" s="3"/>
@@ -4620,23 +6360,41 @@
       <c r="Y75" s="3"/>
     </row>
     <row r="76" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B76" s="18"/>
-      <c r="C76" s="8"/>
-      <c r="D76" s="27"/>
-      <c r="E76" s="10"/>
-      <c r="F76" s="16"/>
-      <c r="G76" s="16"/>
-      <c r="H76" s="16"/>
-      <c r="I76" s="17"/>
+      <c r="B76" s="55">
+        <v>7</v>
+      </c>
+      <c r="C76" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="D76" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E76" s="10">
+        <v>0</v>
+      </c>
+      <c r="F76" s="16">
+        <v>0</v>
+      </c>
+      <c r="G76" s="16">
+        <v>2</v>
+      </c>
+      <c r="H76" s="16">
+        <v>0</v>
+      </c>
+      <c r="I76" s="17">
+        <v>0</v>
+      </c>
       <c r="J76" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K76" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L76" s="8"/>
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="L76" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="M76" s="3"/>
       <c r="N76" s="3"/>
       <c r="O76" s="3"/>
@@ -4652,20 +6410,36 @@
       <c r="Y76" s="3"/>
     </row>
     <row r="77" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B77" s="18"/>
-      <c r="C77" s="8"/>
-      <c r="D77" s="27"/>
-      <c r="E77" s="10"/>
-      <c r="F77" s="16"/>
-      <c r="G77" s="16"/>
-      <c r="H77" s="16"/>
-      <c r="I77" s="17"/>
+      <c r="B77" s="55">
+        <v>7</v>
+      </c>
+      <c r="C77" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="D77" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E77" s="10">
+        <v>0</v>
+      </c>
+      <c r="F77" s="16">
+        <v>0</v>
+      </c>
+      <c r="G77" s="16">
+        <v>0</v>
+      </c>
+      <c r="H77" s="16">
+        <v>1</v>
+      </c>
+      <c r="I77" s="17">
+        <v>0</v>
+      </c>
       <c r="J77" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K77" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L77" s="8"/>
@@ -4684,23 +6458,39 @@
       <c r="Y77" s="3"/>
     </row>
     <row r="78" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B78" s="18"/>
-      <c r="C78" s="8"/>
-      <c r="D78" s="27"/>
-      <c r="E78" s="10"/>
-      <c r="F78" s="16"/>
-      <c r="G78" s="16"/>
-      <c r="H78" s="16"/>
-      <c r="I78" s="17"/>
-      <c r="J78" s="38">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K78" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L78" s="8"/>
+      <c r="B78" s="53">
+        <v>7</v>
+      </c>
+      <c r="C78" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="D78" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="E78" s="47">
+        <v>0</v>
+      </c>
+      <c r="F78" s="48">
+        <v>0</v>
+      </c>
+      <c r="G78" s="48">
+        <v>0</v>
+      </c>
+      <c r="H78" s="48">
+        <v>1</v>
+      </c>
+      <c r="I78" s="49">
+        <v>0</v>
+      </c>
+      <c r="J78" s="50">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K78" s="50">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="L78" s="45"/>
       <c r="M78" s="3"/>
       <c r="N78" s="3"/>
       <c r="O78" s="3"/>
@@ -5397,11 +7187,11 @@
       <c r="H100" s="16"/>
       <c r="I100" s="17"/>
       <c r="J100" s="38">
-        <f t="shared" ref="J100:J111" si="8">IFERROR(F100/(F100+G100),0)</f>
+        <f t="shared" ref="J100:J111" si="12">IFERROR(F100/(F100+G100),0)</f>
         <v>0</v>
       </c>
       <c r="K100" s="38">
-        <f t="shared" ref="K100:K111" si="9">IFERROR(F100/(F100+I100),0)</f>
+        <f t="shared" ref="K100:K111" si="13">IFERROR(F100/(F100+I100),0)</f>
         <v>0</v>
       </c>
       <c r="L100" s="8"/>
@@ -5429,11 +7219,11 @@
       <c r="H101" s="16"/>
       <c r="I101" s="17"/>
       <c r="J101" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K101" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L101" s="8"/>
@@ -5461,11 +7251,11 @@
       <c r="H102" s="16"/>
       <c r="I102" s="17"/>
       <c r="J102" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K102" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L102" s="8"/>
@@ -5493,11 +7283,11 @@
       <c r="H103" s="16"/>
       <c r="I103" s="17"/>
       <c r="J103" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K103" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L103" s="8"/>
@@ -5525,11 +7315,11 @@
       <c r="H104" s="16"/>
       <c r="I104" s="17"/>
       <c r="J104" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K104" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L104" s="8"/>
@@ -5557,11 +7347,11 @@
       <c r="H105" s="16"/>
       <c r="I105" s="17"/>
       <c r="J105" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K105" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L105" s="8"/>
@@ -5589,11 +7379,11 @@
       <c r="H106" s="16"/>
       <c r="I106" s="17"/>
       <c r="J106" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K106" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L106" s="8"/>
@@ -5621,11 +7411,11 @@
       <c r="H107" s="16"/>
       <c r="I107" s="17"/>
       <c r="J107" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K107" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L107" s="8"/>
@@ -5653,11 +7443,11 @@
       <c r="H108" s="16"/>
       <c r="I108" s="17"/>
       <c r="J108" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K108" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L108" s="8"/>
@@ -5685,11 +7475,11 @@
       <c r="H109" s="16"/>
       <c r="I109" s="17"/>
       <c r="J109" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K109" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L109" s="8"/>
@@ -5717,11 +7507,11 @@
       <c r="H110" s="16"/>
       <c r="I110" s="17"/>
       <c r="J110" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K110" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L110" s="8"/>
@@ -5749,11 +7539,11 @@
       <c r="H111" s="16"/>
       <c r="I111" s="17"/>
       <c r="J111" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K111" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L111" s="8"/>

</xml_diff>

<commit_message>
model iteration 8 trained and tests logged
</commit_message>
<xml_diff>
--- a/detection-test-log.xlsx
+++ b/detection-test-log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a00ae3f07a1e700d/Documents/01_Repo/Tennis-Court-Detection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="14_{49F20441-C236-4DE0-9B16-124974D818CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2BD59B5C-CBDB-4676-BE08-4942F2D4DF80}"/>
+  <xr:revisionPtr revIDLastSave="172" documentId="14_{49F20441-C236-4DE0-9B16-124974D818CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D634C8AB-7E17-4F84-9557-6F0ECBBDAFFE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model_Comparison" sheetId="8" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="72">
   <si>
     <t>Comments</t>
   </si>
@@ -234,13 +234,22 @@
     <t>ScaleFactor</t>
   </si>
   <si>
-    <t>Ned to ensure min size &gt; 100 else detects a lot of FP</t>
-  </si>
-  <si>
     <t>Both FPs can be negated with a scaleFactor of 1.5</t>
   </si>
   <si>
     <t>cascade6.xml</t>
+  </si>
+  <si>
+    <t>cascade7.xml</t>
+  </si>
+  <si>
+    <t>Removed 72 low quality pos grey images</t>
+  </si>
+  <si>
+    <t>Set3b</t>
+  </si>
+  <si>
+    <t>Need to ensure min size &gt; 100 else detects a lot of FP</t>
   </si>
 </sst>
 </file>
@@ -740,10 +749,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Model_Comparison!$B$8:$B$14</c:f>
+              <c:f>Model_Comparison!$B$8:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -765,15 +774,18 @@
                 <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Model_Comparison!$Q$8:$Q$14</c:f>
+              <c:f>Model_Comparison!$Q$8:$Q$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
@@ -794,6 +806,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -845,10 +860,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Model_Comparison!$B$8:$B$14</c:f>
+              <c:f>Model_Comparison!$B$8:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -870,15 +885,18 @@
                 <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Model_Comparison!$R$8:$R$14</c:f>
+              <c:f>Model_Comparison!$R$8:$R$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>9.0909090909090912E-2</c:v>
                 </c:pt>
@@ -899,6 +917,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.72727272727272729</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -984,6 +1005,8 @@
         <c:axId val="688872336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="-"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1773,7 +1796,7 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>436033</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>7519</xdr:rowOff>
+      <xdr:rowOff>10694</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2700,7 +2723,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D14" s="30" t="s">
         <v>54</v>
@@ -2771,43 +2794,74 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="32"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="23" t="str">
+      <c r="C15" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="25">
+        <v>244</v>
+      </c>
+      <c r="F15" s="25">
+        <v>255</v>
+      </c>
+      <c r="G15" s="25">
+        <v>1464</v>
+      </c>
+      <c r="H15" s="26">
+        <v>1458</v>
+      </c>
+      <c r="I15" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" s="26">
+        <v>11</v>
+      </c>
+      <c r="K15" s="26">
+        <v>24</v>
+      </c>
+      <c r="L15" s="26">
+        <v>46</v>
+      </c>
+      <c r="M15" s="32">
+        <v>5</v>
+      </c>
+      <c r="N15" s="32">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O15" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="P15" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q15" s="23">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="R15" s="23" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="R15" s="23">
         <f t="shared" si="4"/>
-        <v>-</v>
+        <v>1</v>
       </c>
       <c r="S15" s="22">
         <f>SUMIFS(Test_Logs!F$9:F$113,Test_Logs!$B$9:$B$113,$B15)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="T15" s="22">
         <f>SUMIFS(Test_Logs!G$9:G$113,Test_Logs!$B$9:$B$113,$B15)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="U15" s="22">
         <f>SUMIFS(Test_Logs!H$9:H$113,Test_Logs!$B$9:$B$113,$B15)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="V15" s="22">
         <f>SUMIFS(Test_Logs!I$9:I$113,Test_Logs!$B$9:$B$113,$B15)</f>
         <v>0</v>
+      </c>
+      <c r="W15" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.35">
@@ -3016,10 +3070,10 @@
   <dimension ref="B1:Y147"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="J84" sqref="J84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6343,7 +6397,7 @@
         <v>0</v>
       </c>
       <c r="L75" s="8" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="M75" s="3"/>
       <c r="N75" s="3"/>
@@ -6393,7 +6447,7 @@
         <v>0</v>
       </c>
       <c r="L76" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M76" s="3"/>
       <c r="N76" s="3"/>
@@ -6506,21 +6560,37 @@
       <c r="Y78" s="3"/>
     </row>
     <row r="79" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B79" s="18"/>
-      <c r="C79" s="8"/>
-      <c r="D79" s="27"/>
-      <c r="E79" s="10"/>
-      <c r="F79" s="16"/>
-      <c r="G79" s="16"/>
-      <c r="H79" s="16"/>
-      <c r="I79" s="17"/>
+      <c r="B79" s="55">
+        <v>8</v>
+      </c>
+      <c r="C79" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="D79" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="E79" s="41">
+        <v>3</v>
+      </c>
+      <c r="F79" s="42">
+        <v>3</v>
+      </c>
+      <c r="G79" s="42">
+        <v>0</v>
+      </c>
+      <c r="H79" s="42">
+        <v>3</v>
+      </c>
+      <c r="I79" s="43">
+        <v>0</v>
+      </c>
       <c r="J79" s="38">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" ref="J79:J88" si="12">IFERROR(F79/(F79+G79),0)</f>
+        <v>1</v>
       </c>
       <c r="K79" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" ref="K79:K88" si="13">IFERROR(F79/(F79+I79),0)</f>
+        <v>1</v>
       </c>
       <c r="L79" s="8"/>
       <c r="M79" s="3"/>
@@ -6538,21 +6608,37 @@
       <c r="Y79" s="3"/>
     </row>
     <row r="80" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B80" s="18"/>
-      <c r="C80" s="8"/>
-      <c r="D80" s="27"/>
-      <c r="E80" s="10"/>
-      <c r="F80" s="16"/>
-      <c r="G80" s="16"/>
-      <c r="H80" s="16"/>
-      <c r="I80" s="17"/>
+      <c r="B80" s="55">
+        <v>8</v>
+      </c>
+      <c r="C80" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="D80" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E80" s="10">
+        <v>2</v>
+      </c>
+      <c r="F80" s="16">
+        <v>2</v>
+      </c>
+      <c r="G80" s="16">
+        <v>0</v>
+      </c>
+      <c r="H80" s="16">
+        <v>0</v>
+      </c>
+      <c r="I80" s="17">
+        <v>0</v>
+      </c>
       <c r="J80" s="38">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>1</v>
       </c>
       <c r="K80" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>1</v>
       </c>
       <c r="L80" s="8"/>
       <c r="M80" s="3"/>
@@ -6570,21 +6656,37 @@
       <c r="Y80" s="3"/>
     </row>
     <row r="81" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B81" s="18"/>
-      <c r="C81" s="8"/>
-      <c r="D81" s="27"/>
-      <c r="E81" s="10"/>
-      <c r="F81" s="16"/>
-      <c r="G81" s="16"/>
-      <c r="H81" s="16"/>
-      <c r="I81" s="17"/>
+      <c r="B81" s="55">
+        <v>8</v>
+      </c>
+      <c r="C81" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="D81" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E81" s="10">
+        <v>2</v>
+      </c>
+      <c r="F81" s="16">
+        <v>2</v>
+      </c>
+      <c r="G81" s="16">
+        <v>0</v>
+      </c>
+      <c r="H81" s="16">
+        <v>0</v>
+      </c>
+      <c r="I81" s="17">
+        <v>0</v>
+      </c>
       <c r="J81" s="38">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>1</v>
       </c>
       <c r="K81" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>1</v>
       </c>
       <c r="L81" s="8"/>
       <c r="M81" s="3"/>
@@ -6602,21 +6704,37 @@
       <c r="Y81" s="3"/>
     </row>
     <row r="82" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B82" s="18"/>
-      <c r="C82" s="8"/>
-      <c r="D82" s="27"/>
-      <c r="E82" s="10"/>
-      <c r="F82" s="16"/>
-      <c r="G82" s="16"/>
-      <c r="H82" s="16"/>
-      <c r="I82" s="17"/>
+      <c r="B82" s="55">
+        <v>8</v>
+      </c>
+      <c r="C82" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="D82" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E82" s="10">
+        <v>2</v>
+      </c>
+      <c r="F82" s="16">
+        <v>2</v>
+      </c>
+      <c r="G82" s="16">
+        <v>0</v>
+      </c>
+      <c r="H82" s="16">
+        <v>0</v>
+      </c>
+      <c r="I82" s="17">
+        <v>0</v>
+      </c>
       <c r="J82" s="38">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>1</v>
       </c>
       <c r="K82" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>1</v>
       </c>
       <c r="L82" s="8"/>
       <c r="M82" s="3"/>
@@ -6634,21 +6752,37 @@
       <c r="Y82" s="3"/>
     </row>
     <row r="83" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B83" s="18"/>
-      <c r="C83" s="8"/>
-      <c r="D83" s="27"/>
-      <c r="E83" s="10"/>
-      <c r="F83" s="16"/>
-      <c r="G83" s="16"/>
-      <c r="H83" s="16"/>
-      <c r="I83" s="17"/>
+      <c r="B83" s="55">
+        <v>8</v>
+      </c>
+      <c r="C83" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D83" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E83" s="10">
+        <v>2</v>
+      </c>
+      <c r="F83" s="16">
+        <v>2</v>
+      </c>
+      <c r="G83" s="16">
+        <v>0</v>
+      </c>
+      <c r="H83" s="16">
+        <v>0</v>
+      </c>
+      <c r="I83" s="17">
+        <v>0</v>
+      </c>
       <c r="J83" s="38">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>1</v>
       </c>
       <c r="K83" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>1</v>
       </c>
       <c r="L83" s="8"/>
       <c r="M83" s="3"/>
@@ -6666,20 +6800,36 @@
       <c r="Y83" s="3"/>
     </row>
     <row r="84" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B84" s="18"/>
-      <c r="C84" s="8"/>
-      <c r="D84" s="27"/>
-      <c r="E84" s="10"/>
-      <c r="F84" s="16"/>
-      <c r="G84" s="16"/>
-      <c r="H84" s="16"/>
-      <c r="I84" s="17"/>
+      <c r="B84" s="55">
+        <v>8</v>
+      </c>
+      <c r="C84" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="D84" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E84" s="10">
+        <v>0</v>
+      </c>
+      <c r="F84" s="16">
+        <v>0</v>
+      </c>
+      <c r="G84" s="16">
+        <v>1</v>
+      </c>
+      <c r="H84" s="16">
+        <v>0</v>
+      </c>
+      <c r="I84" s="17">
+        <v>0</v>
+      </c>
       <c r="J84" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K84" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L84" s="8"/>
@@ -6698,23 +6848,41 @@
       <c r="Y84" s="3"/>
     </row>
     <row r="85" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B85" s="18"/>
-      <c r="C85" s="8"/>
-      <c r="D85" s="27"/>
-      <c r="E85" s="10"/>
-      <c r="F85" s="16"/>
-      <c r="G85" s="16"/>
-      <c r="H85" s="16"/>
-      <c r="I85" s="17"/>
+      <c r="B85" s="55">
+        <v>8</v>
+      </c>
+      <c r="C85" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="D85" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E85" s="10">
+        <v>0</v>
+      </c>
+      <c r="F85" s="16">
+        <v>0</v>
+      </c>
+      <c r="G85" s="16">
+        <v>0</v>
+      </c>
+      <c r="H85" s="16">
+        <v>1</v>
+      </c>
+      <c r="I85" s="17">
+        <v>0</v>
+      </c>
       <c r="J85" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K85" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L85" s="8"/>
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="L85" s="8" t="s">
+        <v>71</v>
+      </c>
       <c r="M85" s="3"/>
       <c r="N85" s="3"/>
       <c r="O85" s="3"/>
@@ -6730,20 +6898,36 @@
       <c r="Y85" s="3"/>
     </row>
     <row r="86" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B86" s="18"/>
-      <c r="C86" s="8"/>
-      <c r="D86" s="27"/>
-      <c r="E86" s="10"/>
-      <c r="F86" s="16"/>
-      <c r="G86" s="16"/>
-      <c r="H86" s="16"/>
-      <c r="I86" s="17"/>
+      <c r="B86" s="55">
+        <v>8</v>
+      </c>
+      <c r="C86" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="D86" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E86" s="10">
+        <v>0</v>
+      </c>
+      <c r="F86" s="16">
+        <v>0</v>
+      </c>
+      <c r="G86" s="16">
+        <v>10</v>
+      </c>
+      <c r="H86" s="16">
+        <v>0</v>
+      </c>
+      <c r="I86" s="17">
+        <v>0</v>
+      </c>
       <c r="J86" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K86" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L86" s="8"/>
@@ -6762,20 +6946,36 @@
       <c r="Y86" s="3"/>
     </row>
     <row r="87" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B87" s="18"/>
-      <c r="C87" s="8"/>
-      <c r="D87" s="27"/>
-      <c r="E87" s="10"/>
-      <c r="F87" s="16"/>
-      <c r="G87" s="16"/>
-      <c r="H87" s="16"/>
-      <c r="I87" s="17"/>
+      <c r="B87" s="55">
+        <v>8</v>
+      </c>
+      <c r="C87" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="D87" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E87" s="10">
+        <v>0</v>
+      </c>
+      <c r="F87" s="16">
+        <v>0</v>
+      </c>
+      <c r="G87" s="16">
+        <v>0</v>
+      </c>
+      <c r="H87" s="16">
+        <v>1</v>
+      </c>
+      <c r="I87" s="17">
+        <v>0</v>
+      </c>
       <c r="J87" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K87" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L87" s="8"/>
@@ -6794,23 +6994,39 @@
       <c r="Y87" s="3"/>
     </row>
     <row r="88" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B88" s="18"/>
-      <c r="C88" s="8"/>
-      <c r="D88" s="27"/>
-      <c r="E88" s="10"/>
-      <c r="F88" s="16"/>
-      <c r="G88" s="16"/>
-      <c r="H88" s="16"/>
-      <c r="I88" s="17"/>
-      <c r="J88" s="38">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K88" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L88" s="8"/>
+      <c r="B88" s="53">
+        <v>8</v>
+      </c>
+      <c r="C88" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="D88" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="E88" s="47">
+        <v>0</v>
+      </c>
+      <c r="F88" s="48">
+        <v>0</v>
+      </c>
+      <c r="G88" s="48">
+        <v>0</v>
+      </c>
+      <c r="H88" s="48">
+        <v>1</v>
+      </c>
+      <c r="I88" s="49">
+        <v>0</v>
+      </c>
+      <c r="J88" s="50">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K88" s="50">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="L88" s="45"/>
       <c r="M88" s="3"/>
       <c r="N88" s="3"/>
       <c r="O88" s="3"/>
@@ -7187,11 +7403,11 @@
       <c r="H100" s="16"/>
       <c r="I100" s="17"/>
       <c r="J100" s="38">
-        <f t="shared" ref="J100:J111" si="12">IFERROR(F100/(F100+G100),0)</f>
+        <f t="shared" ref="J100:J111" si="14">IFERROR(F100/(F100+G100),0)</f>
         <v>0</v>
       </c>
       <c r="K100" s="38">
-        <f t="shared" ref="K100:K111" si="13">IFERROR(F100/(F100+I100),0)</f>
+        <f t="shared" ref="K100:K111" si="15">IFERROR(F100/(F100+I100),0)</f>
         <v>0</v>
       </c>
       <c r="L100" s="8"/>
@@ -7219,11 +7435,11 @@
       <c r="H101" s="16"/>
       <c r="I101" s="17"/>
       <c r="J101" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K101" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L101" s="8"/>
@@ -7251,11 +7467,11 @@
       <c r="H102" s="16"/>
       <c r="I102" s="17"/>
       <c r="J102" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K102" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L102" s="8"/>
@@ -7283,11 +7499,11 @@
       <c r="H103" s="16"/>
       <c r="I103" s="17"/>
       <c r="J103" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K103" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L103" s="8"/>
@@ -7315,11 +7531,11 @@
       <c r="H104" s="16"/>
       <c r="I104" s="17"/>
       <c r="J104" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K104" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L104" s="8"/>
@@ -7347,11 +7563,11 @@
       <c r="H105" s="16"/>
       <c r="I105" s="17"/>
       <c r="J105" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K105" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L105" s="8"/>
@@ -7379,11 +7595,11 @@
       <c r="H106" s="16"/>
       <c r="I106" s="17"/>
       <c r="J106" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K106" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L106" s="8"/>
@@ -7411,11 +7627,11 @@
       <c r="H107" s="16"/>
       <c r="I107" s="17"/>
       <c r="J107" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K107" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L107" s="8"/>
@@ -7443,11 +7659,11 @@
       <c r="H108" s="16"/>
       <c r="I108" s="17"/>
       <c r="J108" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K108" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L108" s="8"/>
@@ -7475,11 +7691,11 @@
       <c r="H109" s="16"/>
       <c r="I109" s="17"/>
       <c r="J109" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K109" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L109" s="8"/>
@@ -7507,11 +7723,11 @@
       <c r="H110" s="16"/>
       <c r="I110" s="17"/>
       <c r="J110" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K110" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L110" s="8"/>
@@ -7539,11 +7755,11 @@
       <c r="H111" s="16"/>
       <c r="I111" s="17"/>
       <c r="J111" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K111" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L111" s="8"/>

</xml_diff>

<commit_message>
Updated with new trained model (cascade8)
</commit_message>
<xml_diff>
--- a/detection-test-log.xlsx
+++ b/detection-test-log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a00ae3f07a1e700d/Documents/01_Repo/Tennis-Court-Detection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="172" documentId="14_{49F20441-C236-4DE0-9B16-124974D818CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D634C8AB-7E17-4F84-9557-6F0ECBBDAFFE}"/>
+  <xr:revisionPtr revIDLastSave="210" documentId="14_{49F20441-C236-4DE0-9B16-124974D818CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B6B6CE3A-7E3D-477A-85B8-45CF46FD76B1}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model_Comparison" sheetId="8" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="74">
   <si>
     <t>Comments</t>
   </si>
@@ -228,9 +228,6 @@
     <t>LBP</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>ScaleFactor</t>
   </si>
   <si>
@@ -250,6 +247,15 @@
   </si>
   <si>
     <t>Need to ensure min size &gt; 100 else detects a lot of FP</t>
+  </si>
+  <si>
+    <t>Set4</t>
+  </si>
+  <si>
+    <t>manual</t>
+  </si>
+  <si>
+    <t>Negatives rotated at 0, 180. (pos -2, 0, 2, 178, 180, 182). Pos img 90%. Image dimensions 60 x 114. Removed some low quality images from Set3b (and earlier)</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1012,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
-          <c:min val="-"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2235,7 +2241,7 @@
         <v>40</v>
       </c>
       <c r="N7" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O7" s="33" t="s">
         <v>45</v>
@@ -2687,7 +2693,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="O13" s="32" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="P13" s="32" t="s">
         <v>50</v>
@@ -2723,7 +2729,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D14" s="30" t="s">
         <v>54</v>
@@ -2759,7 +2765,7 @@
         <v>1.2</v>
       </c>
       <c r="O14" s="32" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="P14" s="32" t="s">
         <v>50</v>
@@ -2795,10 +2801,10 @@
         <v>8</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E15" s="25">
         <v>244</v>
@@ -2831,7 +2837,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="O15" s="32" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="P15" s="32" t="s">
         <v>50</v>
@@ -2861,7 +2867,7 @@
         <v>0</v>
       </c>
       <c r="W15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.35">
@@ -2870,15 +2876,31 @@
         <v>9</v>
       </c>
       <c r="C16" s="15"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
+      <c r="D16" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="25">
+        <v>916</v>
+      </c>
+      <c r="F16" s="25">
+        <v>365</v>
+      </c>
+      <c r="G16" s="25">
+        <v>1830</v>
+      </c>
+      <c r="H16" s="26">
+        <v>2190</v>
+      </c>
+      <c r="I16" s="26" t="s">
+        <v>63</v>
+      </c>
       <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
+      <c r="K16" s="26">
+        <v>24</v>
+      </c>
+      <c r="L16" s="26">
+        <v>46</v>
+      </c>
       <c r="M16" s="32"/>
       <c r="N16" s="32"/>
       <c r="O16" s="32"/>
@@ -2906,6 +2928,9 @@
       <c r="V16" s="22">
         <f>SUMIFS(Test_Logs!I$9:I$113,Test_Logs!$B$9:$B$113,$B16)</f>
         <v>0</v>
+      </c>
+      <c r="X16" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.35">
@@ -6397,7 +6422,7 @@
         <v>0</v>
       </c>
       <c r="L75" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M75" s="3"/>
       <c r="N75" s="3"/>
@@ -6447,7 +6472,7 @@
         <v>0</v>
       </c>
       <c r="L76" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M76" s="3"/>
       <c r="N76" s="3"/>
@@ -6881,7 +6906,7 @@
         <v>0</v>
       </c>
       <c r="L85" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M85" s="3"/>
       <c r="N85" s="3"/>

</xml_diff>

<commit_message>
model iteration 9 tests logged
</commit_message>
<xml_diff>
--- a/detection-test-log.xlsx
+++ b/detection-test-log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a00ae3f07a1e700d/Documents/01_Repo/Tennis-Court-Detection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="210" documentId="14_{49F20441-C236-4DE0-9B16-124974D818CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B6B6CE3A-7E3D-477A-85B8-45CF46FD76B1}"/>
+  <xr:revisionPtr revIDLastSave="249" documentId="14_{49F20441-C236-4DE0-9B16-124974D818CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8A9EE360-A6D0-45E5-8145-90BC80F50B73}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model_Comparison" sheetId="8" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="76">
   <si>
     <t>Comments</t>
   </si>
@@ -255,7 +255,13 @@
     <t>manual</t>
   </si>
   <si>
-    <t>Negatives rotated at 0, 180. (pos -2, 0, 2, 178, 180, 182). Pos img 90%. Image dimensions 60 x 114. Removed some low quality images from Set3b (and earlier)</t>
+    <t>cascade8.xml</t>
+  </si>
+  <si>
+    <t>Negatives rotated at 0, 180. (pos -2, 0, 2, 178, 180, 182). Pos img 90%. Image dimensions 60 x 114. Removed some low quality (original colour) images from Set3b (and earlier)</t>
+  </si>
+  <si>
+    <t>FP was overlapping on the tennis court</t>
   </si>
 </sst>
 </file>
@@ -755,10 +761,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Model_Comparison!$B$8:$B$15</c:f>
+              <c:f>Model_Comparison!$B$8:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -783,15 +789,18 @@
                 <c:pt idx="7">
                   <c:v>8</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Model_Comparison!$Q$8:$Q$15</c:f>
+              <c:f>Model_Comparison!$Q$8:$Q$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
@@ -815,6 +824,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.90909090909090906</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -866,10 +878,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Model_Comparison!$B$8:$B$15</c:f>
+              <c:f>Model_Comparison!$B$8:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -894,15 +906,18 @@
                 <c:pt idx="7">
                   <c:v>8</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Model_Comparison!$R$8:$R$15</c:f>
+              <c:f>Model_Comparison!$R$8:$R$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>9.0909090909090912E-2</c:v>
                 </c:pt>
@@ -926,6 +941,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.90909090909090906</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -952,6 +970,7 @@
         <c:axId val="688870096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -969,6 +988,78 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1300" b="1">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Model</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1300" b="1" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> Iteration</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA" sz="1300" b="1">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1758,10 +1849,10 @@
       <xdr:rowOff>41273</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1003300</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:rowOff>146049</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2875,7 +2966,9 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="C16" s="15"/>
+      <c r="C16" s="15" t="s">
+        <v>73</v>
+      </c>
       <c r="D16" s="30" t="s">
         <v>71</v>
       </c>
@@ -2901,36 +2994,44 @@
       <c r="L16" s="26">
         <v>46</v>
       </c>
-      <c r="M16" s="32"/>
-      <c r="N16" s="32"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="23" t="str">
+      <c r="M16" s="32">
+        <v>5</v>
+      </c>
+      <c r="N16" s="32">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O16" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="P16" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q16" s="23">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="R16" s="23" t="str">
+        <v>0.90909090909090906</v>
+      </c>
+      <c r="R16" s="23">
         <f t="shared" si="4"/>
-        <v>-</v>
+        <v>0.90909090909090906</v>
       </c>
       <c r="S16" s="22">
         <f>SUMIFS(Test_Logs!F$9:F$113,Test_Logs!$B$9:$B$113,$B16)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="T16" s="22">
         <f>SUMIFS(Test_Logs!G$9:G$113,Test_Logs!$B$9:$B$113,$B16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U16" s="22">
         <f>SUMIFS(Test_Logs!H$9:H$113,Test_Logs!$B$9:$B$113,$B16)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="V16" s="22">
         <f>SUMIFS(Test_Logs!I$9:I$113,Test_Logs!$B$9:$B$113,$B16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.35">
@@ -3082,6 +3183,7 @@
       <c r="M26" s="57"/>
       <c r="N26" s="57"/>
       <c r="O26" s="57"/>
+      <c r="P26" s="57"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3095,10 +3197,10 @@
   <dimension ref="B1:Y147"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="B63" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="J84" sqref="J84"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7067,21 +7169,37 @@
       <c r="Y88" s="3"/>
     </row>
     <row r="89" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B89" s="18"/>
-      <c r="C89" s="8"/>
-      <c r="D89" s="27"/>
-      <c r="E89" s="10"/>
-      <c r="F89" s="16"/>
-      <c r="G89" s="16"/>
-      <c r="H89" s="16"/>
-      <c r="I89" s="17"/>
+      <c r="B89" s="55">
+        <v>9</v>
+      </c>
+      <c r="C89" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="D89" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="E89" s="41">
+        <v>3</v>
+      </c>
+      <c r="F89" s="42">
+        <v>3</v>
+      </c>
+      <c r="G89" s="42">
+        <v>0</v>
+      </c>
+      <c r="H89" s="42">
+        <v>3</v>
+      </c>
+      <c r="I89" s="43">
+        <v>0</v>
+      </c>
       <c r="J89" s="38">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" ref="J89:J98" si="14">IFERROR(F89/(F89+G89),0)</f>
+        <v>1</v>
       </c>
       <c r="K89" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" ref="K89:K98" si="15">IFERROR(F89/(F89+I89),0)</f>
+        <v>1</v>
       </c>
       <c r="L89" s="8"/>
       <c r="M89" s="3"/>
@@ -7099,21 +7217,37 @@
       <c r="Y89" s="3"/>
     </row>
     <row r="90" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B90" s="18"/>
-      <c r="C90" s="8"/>
-      <c r="D90" s="27"/>
-      <c r="E90" s="10"/>
-      <c r="F90" s="16"/>
-      <c r="G90" s="16"/>
-      <c r="H90" s="16"/>
-      <c r="I90" s="17"/>
+      <c r="B90" s="55">
+        <v>9</v>
+      </c>
+      <c r="C90" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="D90" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E90" s="10">
+        <v>2</v>
+      </c>
+      <c r="F90" s="16">
+        <v>1</v>
+      </c>
+      <c r="G90" s="16">
+        <v>0</v>
+      </c>
+      <c r="H90" s="16">
+        <v>0</v>
+      </c>
+      <c r="I90" s="17">
+        <v>1</v>
+      </c>
       <c r="J90" s="38">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>1</v>
       </c>
       <c r="K90" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>0.5</v>
       </c>
       <c r="L90" s="8"/>
       <c r="M90" s="3"/>
@@ -7131,23 +7265,41 @@
       <c r="Y90" s="3"/>
     </row>
     <row r="91" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B91" s="18"/>
-      <c r="C91" s="8"/>
-      <c r="D91" s="27"/>
-      <c r="E91" s="10"/>
-      <c r="F91" s="16"/>
-      <c r="G91" s="16"/>
-      <c r="H91" s="16"/>
-      <c r="I91" s="17"/>
+      <c r="B91" s="55">
+        <v>9</v>
+      </c>
+      <c r="C91" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="D91" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E91" s="10">
+        <v>2</v>
+      </c>
+      <c r="F91" s="16">
+        <v>2</v>
+      </c>
+      <c r="G91" s="16">
+        <v>1</v>
+      </c>
+      <c r="H91" s="16">
+        <v>0</v>
+      </c>
+      <c r="I91" s="17">
+        <v>0</v>
+      </c>
       <c r="J91" s="38">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="K91" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L91" s="8"/>
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="L91" s="8" t="s">
+        <v>75</v>
+      </c>
       <c r="M91" s="3"/>
       <c r="N91" s="3"/>
       <c r="O91" s="3"/>
@@ -7163,21 +7315,37 @@
       <c r="Y91" s="3"/>
     </row>
     <row r="92" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B92" s="18"/>
-      <c r="C92" s="8"/>
-      <c r="D92" s="27"/>
-      <c r="E92" s="10"/>
-      <c r="F92" s="16"/>
-      <c r="G92" s="16"/>
-      <c r="H92" s="16"/>
-      <c r="I92" s="17"/>
+      <c r="B92" s="55">
+        <v>9</v>
+      </c>
+      <c r="C92" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="D92" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E92" s="10">
+        <v>2</v>
+      </c>
+      <c r="F92" s="16">
+        <v>2</v>
+      </c>
+      <c r="G92" s="16">
+        <v>0</v>
+      </c>
+      <c r="H92" s="16">
+        <v>0</v>
+      </c>
+      <c r="I92" s="17">
+        <v>0</v>
+      </c>
       <c r="J92" s="38">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>1</v>
       </c>
       <c r="K92" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>1</v>
       </c>
       <c r="L92" s="8"/>
       <c r="M92" s="3"/>
@@ -7195,21 +7363,37 @@
       <c r="Y92" s="3"/>
     </row>
     <row r="93" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B93" s="18"/>
-      <c r="C93" s="8"/>
-      <c r="D93" s="27"/>
-      <c r="E93" s="10"/>
-      <c r="F93" s="16"/>
-      <c r="G93" s="16"/>
-      <c r="H93" s="16"/>
-      <c r="I93" s="17"/>
+      <c r="B93" s="55">
+        <v>9</v>
+      </c>
+      <c r="C93" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D93" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E93" s="10">
+        <v>2</v>
+      </c>
+      <c r="F93" s="16">
+        <v>2</v>
+      </c>
+      <c r="G93" s="16">
+        <v>0</v>
+      </c>
+      <c r="H93" s="16">
+        <v>0</v>
+      </c>
+      <c r="I93" s="17">
+        <v>0</v>
+      </c>
       <c r="J93" s="38">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>1</v>
       </c>
       <c r="K93" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>1</v>
       </c>
       <c r="L93" s="8"/>
       <c r="M93" s="3"/>
@@ -7227,20 +7411,36 @@
       <c r="Y93" s="3"/>
     </row>
     <row r="94" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B94" s="18"/>
-      <c r="C94" s="8"/>
-      <c r="D94" s="27"/>
-      <c r="E94" s="10"/>
-      <c r="F94" s="16"/>
-      <c r="G94" s="16"/>
-      <c r="H94" s="16"/>
-      <c r="I94" s="17"/>
+      <c r="B94" s="55">
+        <v>9</v>
+      </c>
+      <c r="C94" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="D94" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E94" s="10">
+        <v>0</v>
+      </c>
+      <c r="F94" s="16">
+        <v>0</v>
+      </c>
+      <c r="G94" s="16">
+        <v>0</v>
+      </c>
+      <c r="H94" s="16">
+        <v>1</v>
+      </c>
+      <c r="I94" s="17">
+        <v>0</v>
+      </c>
       <c r="J94" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K94" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L94" s="8"/>
@@ -7259,23 +7459,41 @@
       <c r="Y94" s="3"/>
     </row>
     <row r="95" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B95" s="18"/>
-      <c r="C95" s="8"/>
-      <c r="D95" s="27"/>
-      <c r="E95" s="10"/>
-      <c r="F95" s="16"/>
-      <c r="G95" s="16"/>
-      <c r="H95" s="16"/>
-      <c r="I95" s="17"/>
+      <c r="B95" s="55">
+        <v>9</v>
+      </c>
+      <c r="C95" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="D95" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E95" s="10">
+        <v>0</v>
+      </c>
+      <c r="F95" s="16">
+        <v>0</v>
+      </c>
+      <c r="G95" s="16">
+        <v>0</v>
+      </c>
+      <c r="H95" s="16">
+        <v>1</v>
+      </c>
+      <c r="I95" s="17">
+        <v>0</v>
+      </c>
       <c r="J95" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K95" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L95" s="8"/>
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="L95" s="8" t="s">
+        <v>70</v>
+      </c>
       <c r="M95" s="3"/>
       <c r="N95" s="3"/>
       <c r="O95" s="3"/>
@@ -7291,20 +7509,36 @@
       <c r="Y95" s="3"/>
     </row>
     <row r="96" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B96" s="18"/>
-      <c r="C96" s="8"/>
-      <c r="D96" s="27"/>
-      <c r="E96" s="10"/>
-      <c r="F96" s="16"/>
-      <c r="G96" s="16"/>
-      <c r="H96" s="16"/>
-      <c r="I96" s="17"/>
+      <c r="B96" s="55">
+        <v>9</v>
+      </c>
+      <c r="C96" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="D96" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E96" s="10">
+        <v>0</v>
+      </c>
+      <c r="F96" s="16">
+        <v>0</v>
+      </c>
+      <c r="G96" s="16">
+        <v>0</v>
+      </c>
+      <c r="H96" s="16">
+        <v>1</v>
+      </c>
+      <c r="I96" s="17">
+        <v>0</v>
+      </c>
       <c r="J96" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K96" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L96" s="8"/>
@@ -7323,20 +7557,36 @@
       <c r="Y96" s="3"/>
     </row>
     <row r="97" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B97" s="18"/>
-      <c r="C97" s="8"/>
-      <c r="D97" s="27"/>
-      <c r="E97" s="10"/>
-      <c r="F97" s="16"/>
-      <c r="G97" s="16"/>
-      <c r="H97" s="16"/>
-      <c r="I97" s="17"/>
+      <c r="B97" s="55">
+        <v>9</v>
+      </c>
+      <c r="C97" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="D97" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E97" s="10">
+        <v>0</v>
+      </c>
+      <c r="F97" s="16">
+        <v>0</v>
+      </c>
+      <c r="G97" s="16">
+        <v>0</v>
+      </c>
+      <c r="H97" s="16">
+        <v>1</v>
+      </c>
+      <c r="I97" s="17">
+        <v>0</v>
+      </c>
       <c r="J97" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K97" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L97" s="8"/>
@@ -7355,23 +7605,39 @@
       <c r="Y97" s="3"/>
     </row>
     <row r="98" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B98" s="18"/>
-      <c r="C98" s="8"/>
-      <c r="D98" s="27"/>
-      <c r="E98" s="10"/>
-      <c r="F98" s="16"/>
-      <c r="G98" s="16"/>
-      <c r="H98" s="16"/>
-      <c r="I98" s="17"/>
-      <c r="J98" s="38">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K98" s="38">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L98" s="8"/>
+      <c r="B98" s="53">
+        <v>9</v>
+      </c>
+      <c r="C98" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="D98" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="E98" s="47">
+        <v>0</v>
+      </c>
+      <c r="F98" s="48">
+        <v>0</v>
+      </c>
+      <c r="G98" s="48">
+        <v>0</v>
+      </c>
+      <c r="H98" s="48">
+        <v>1</v>
+      </c>
+      <c r="I98" s="49">
+        <v>0</v>
+      </c>
+      <c r="J98" s="50">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="K98" s="50">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="L98" s="45"/>
       <c r="M98" s="3"/>
       <c r="N98" s="3"/>
       <c r="O98" s="3"/>
@@ -7428,11 +7694,11 @@
       <c r="H100" s="16"/>
       <c r="I100" s="17"/>
       <c r="J100" s="38">
-        <f t="shared" ref="J100:J111" si="14">IFERROR(F100/(F100+G100),0)</f>
+        <f t="shared" ref="J100:J111" si="16">IFERROR(F100/(F100+G100),0)</f>
         <v>0</v>
       </c>
       <c r="K100" s="38">
-        <f t="shared" ref="K100:K111" si="15">IFERROR(F100/(F100+I100),0)</f>
+        <f t="shared" ref="K100:K111" si="17">IFERROR(F100/(F100+I100),0)</f>
         <v>0</v>
       </c>
       <c r="L100" s="8"/>
@@ -7460,11 +7726,11 @@
       <c r="H101" s="16"/>
       <c r="I101" s="17"/>
       <c r="J101" s="38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="K101" s="38">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L101" s="8"/>
@@ -7492,11 +7758,11 @@
       <c r="H102" s="16"/>
       <c r="I102" s="17"/>
       <c r="J102" s="38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="K102" s="38">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L102" s="8"/>
@@ -7524,11 +7790,11 @@
       <c r="H103" s="16"/>
       <c r="I103" s="17"/>
       <c r="J103" s="38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="K103" s="38">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L103" s="8"/>
@@ -7556,11 +7822,11 @@
       <c r="H104" s="16"/>
       <c r="I104" s="17"/>
       <c r="J104" s="38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="K104" s="38">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L104" s="8"/>
@@ -7588,11 +7854,11 @@
       <c r="H105" s="16"/>
       <c r="I105" s="17"/>
       <c r="J105" s="38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="K105" s="38">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L105" s="8"/>
@@ -7620,11 +7886,11 @@
       <c r="H106" s="16"/>
       <c r="I106" s="17"/>
       <c r="J106" s="38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="K106" s="38">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L106" s="8"/>
@@ -7652,11 +7918,11 @@
       <c r="H107" s="16"/>
       <c r="I107" s="17"/>
       <c r="J107" s="38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="K107" s="38">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L107" s="8"/>
@@ -7684,11 +7950,11 @@
       <c r="H108" s="16"/>
       <c r="I108" s="17"/>
       <c r="J108" s="38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="K108" s="38">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L108" s="8"/>
@@ -7716,11 +7982,11 @@
       <c r="H109" s="16"/>
       <c r="I109" s="17"/>
       <c r="J109" s="38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="K109" s="38">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L109" s="8"/>
@@ -7748,11 +8014,11 @@
       <c r="H110" s="16"/>
       <c r="I110" s="17"/>
       <c r="J110" s="38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="K110" s="38">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L110" s="8"/>
@@ -7780,11 +8046,11 @@
       <c r="H111" s="16"/>
       <c r="I111" s="17"/>
       <c r="J111" s="38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="K111" s="38">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L111" s="8"/>

</xml_diff>